<commit_message>
Se modifico el cronograma
</commit_message>
<xml_diff>
--- a/assets/Trimestres/Trimestre_3/Cronograma TPS_2926378_V2.xlsx
+++ b/assets/Trimestres/Trimestre_3/Cronograma TPS_2926378_V2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC46C55E-A17D-40E6-9AC3-005EFB6C033E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F660B35-B272-4127-BF62-6BA4E2D49A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" xr2:uid="{2EF96F3D-4256-48DD-8CAA-143A5EBF2E06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="241">
   <si>
     <t>Cronograma de Actividades</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>&lt;Nombre del Proyecto&gt;</t>
   </si>
   <si>
     <t>Inventario</t>
@@ -2816,24 +2813,61 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2843,7 +2877,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2854,83 +2887,23 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="79" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2940,16 +2913,40 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="21" fillId="0" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="79" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3034,7 +3031,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{211C1BEE-9002-CDE9-8A84-900732D0DFCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3252,79 +3249,25 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="432000" cy="432000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="76201" y="104776"/>
-          <a:ext cx="432000" cy="432000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln cap="flat">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>114301</xdr:colOff>
+      <xdr:colOff>130969</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>608803</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>173033</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:rowOff>223837</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B784D8FC-914F-83DC-0971-3724F7996866}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E2F676-5181-46E1-B29F-3231EDE58040}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3340,7 +3283,70 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="114301" y="57150"/>
+          <a:off x="130969" y="59531"/>
+          <a:ext cx="494502" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>561178</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66676" y="85725"/>
           <a:ext cx="494502" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3436,7 +3442,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5683881F-354A-4316-87AD-246A172D3B73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3535,20 +3541,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>561177</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{843247C8-D48A-47BB-95E3-345E324D7E60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3564,7 +3570,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66675" y="95250"/>
+          <a:off x="66675" y="66675"/>
           <a:ext cx="494502" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3660,7 +3666,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7956611E-8E11-4A0F-9FF5-222C1BD78917}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3993,7 +3999,7 @@
   <dimension ref="A2:P82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
@@ -4015,121 +4021,121 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="182" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
+      <c r="B3" s="168" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="182" t="s">
+      <c r="B4" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="182"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="183"/>
-      <c r="C5" s="183"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
+      <c r="B5" s="169"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="3"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="170" t="s">
+      <c r="B8" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="170"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="170"/>
-      <c r="F8" s="170"/>
+      <c r="C8" s="197"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="191" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="192"/>
-      <c r="E11" s="192"/>
-      <c r="F11" s="193"/>
+      <c r="C11" s="178" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="179"/>
+      <c r="E11" s="179"/>
+      <c r="F11" s="180"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="168" t="s">
-        <v>235</v>
-      </c>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
-      <c r="F12" s="195"/>
+      <c r="C12" s="181" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" s="182"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="183"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="168" t="s">
+      <c r="C13" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="194"/>
-      <c r="E13" s="196"/>
-      <c r="F13" s="195"/>
+      <c r="D13" s="182"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="183"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="168" t="s">
-        <v>236</v>
-      </c>
-      <c r="D14" s="169"/>
+      <c r="C14" s="181" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="196"/>
       <c r="E14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="19.899999999999999" customHeight="1">
       <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="197" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="198"/>
+      <c r="C15" s="185" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="186"/>
       <c r="E15" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="199" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="200"/>
+      <c r="C16" s="187" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="188"/>
       <c r="E16" s="30" t="s">
         <v>10</v>
       </c>
@@ -4139,8 +4145,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="4"/>
-      <c r="C17" s="188"/>
-      <c r="D17" s="188"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="174"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -4159,27 +4165,27 @@
       <c r="C21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="189" t="s">
+      <c r="D21" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="189"/>
+      <c r="E21" s="175"/>
       <c r="F21" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="190" t="s">
+      <c r="D22" s="176" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="176"/>
+      <c r="F22" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="E22" s="190"/>
-      <c r="F22" s="20" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
@@ -4234,8 +4240,8 @@
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="178"/>
-      <c r="E30" s="178"/>
+      <c r="D30" s="192"/>
+      <c r="E30" s="192"/>
       <c r="F30" s="26"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -4246,61 +4252,61 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="179" t="s">
+      <c r="B34" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="180"/>
-      <c r="D34" s="180"/>
-      <c r="E34" s="180"/>
-      <c r="F34" s="181"/>
+      <c r="C34" s="194"/>
+      <c r="D34" s="194"/>
+      <c r="E34" s="194"/>
+      <c r="F34" s="195"/>
     </row>
     <row r="35" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="185" t="s">
+      <c r="B35" s="171" t="s">
+        <v>235</v>
+      </c>
+      <c r="C35" s="172"/>
+      <c r="D35" s="172"/>
+      <c r="E35" s="172"/>
+      <c r="F35" s="173"/>
+    </row>
+    <row r="36" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B36" s="198" t="s">
         <v>236</v>
       </c>
-      <c r="C35" s="186"/>
-      <c r="D35" s="186"/>
-      <c r="E35" s="186"/>
-      <c r="F35" s="187"/>
-    </row>
-    <row r="36" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="171" t="s">
-        <v>237</v>
-      </c>
-      <c r="C36" s="172"/>
-      <c r="D36" s="172"/>
-      <c r="E36" s="172"/>
-      <c r="F36" s="173"/>
+      <c r="C36" s="199"/>
+      <c r="D36" s="199"/>
+      <c r="E36" s="199"/>
+      <c r="F36" s="200"/>
       <c r="J36" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="171" t="s">
+      <c r="B37" s="198" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="199"/>
+      <c r="D37" s="199"/>
+      <c r="E37" s="199"/>
+      <c r="F37" s="200"/>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B38" s="198" t="s">
         <v>238</v>
       </c>
-      <c r="C37" s="172"/>
-      <c r="D37" s="172"/>
-      <c r="E37" s="172"/>
-      <c r="F37" s="173"/>
-    </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="171" t="s">
+      <c r="C38" s="199"/>
+      <c r="D38" s="199"/>
+      <c r="E38" s="199"/>
+      <c r="F38" s="200"/>
+    </row>
+    <row r="39" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B39" s="189" t="s">
         <v>239</v>
       </c>
-      <c r="C38" s="172"/>
-      <c r="D38" s="172"/>
-      <c r="E38" s="172"/>
-      <c r="F38" s="173"/>
-    </row>
-    <row r="39" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="174" t="s">
-        <v>240</v>
-      </c>
-      <c r="C39" s="175"/>
-      <c r="D39" s="175"/>
-      <c r="E39" s="175"/>
-      <c r="F39" s="176"/>
+      <c r="C39" s="190"/>
+      <c r="D39" s="190"/>
+      <c r="E39" s="190"/>
+      <c r="F39" s="191"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="7"/>
@@ -4461,6 +4467,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
@@ -4477,18 +4495,6 @@
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -4505,7 +4511,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4520,22 +4526,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="148" customFormat="1" ht="24.95" customHeight="1">
       <c r="A1" s="149" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="150" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="150" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="150" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="150" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="150" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="150" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="150" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="150" t="s">
+      <c r="F1" s="151" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="151" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="76" customFormat="1" ht="9.9499999999999993" customHeight="1">
@@ -4551,10 +4557,10 @@
         <v>220501092</v>
       </c>
       <c r="B3" s="143" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="144" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="145"/>
       <c r="E3" s="145"/>
@@ -4568,16 +4574,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="77" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="77" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="76" customFormat="1" ht="39.950000000000003" customHeight="1">
@@ -4588,16 +4594,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="76" customFormat="1" ht="39.950000000000003" customHeight="1">
@@ -4608,10 +4614,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" s="79"/>
       <c r="F6" s="79"/>
@@ -4624,10 +4630,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="79"/>
       <c r="F7" s="79"/>
@@ -4640,10 +4646,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" s="79"/>
       <c r="F8" s="79"/>
@@ -4664,16 +4670,16 @@
         <v>2</v>
       </c>
       <c r="C10" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="77" t="s">
-        <v>66</v>
-      </c>
       <c r="E10" s="77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -4684,16 +4690,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -4704,13 +4710,13 @@
         <v>2</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="77" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="79"/>
     </row>
@@ -4722,10 +4728,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="79"/>
       <c r="F13" s="79"/>
@@ -4738,10 +4744,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="79"/>
       <c r="F14" s="79"/>
@@ -4754,10 +4760,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="79"/>
       <c r="F15" s="79"/>
@@ -4770,10 +4776,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="77" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
@@ -4786,10 +4792,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="79"/>
       <c r="F17" s="79"/>
@@ -4802,10 +4808,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18" s="79"/>
       <c r="F18" s="79"/>
@@ -4818,10 +4824,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E19" s="79"/>
       <c r="F19" s="79"/>
@@ -4834,10 +4840,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="79"/>
       <c r="F20" s="79"/>
@@ -4850,10 +4856,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" s="79"/>
       <c r="F21" s="79"/>
@@ -4866,10 +4872,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="79"/>
       <c r="F22" s="79"/>
@@ -4882,10 +4888,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="79"/>
       <c r="F23" s="79"/>
@@ -4903,10 +4909,10 @@
         <v>220501113</v>
       </c>
       <c r="B25" s="143" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="144" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="145"/>
       <c r="E25" s="145"/>
@@ -4920,16 +4926,16 @@
         <v>1</v>
       </c>
       <c r="C26" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="77" t="s">
-        <v>84</v>
-      </c>
       <c r="E26" s="77" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" s="77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="51">
@@ -4940,13 +4946,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27" s="77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" s="79"/>
     </row>
@@ -4958,10 +4964,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E28" s="79"/>
       <c r="F28" s="79"/>
@@ -4974,10 +4980,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29" s="79"/>
       <c r="F29" s="79"/>
@@ -4990,10 +4996,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30" s="77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E30" s="79"/>
       <c r="F30" s="79"/>
@@ -5006,10 +5012,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D31" s="77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="79"/>
       <c r="F31" s="79"/>
@@ -5022,10 +5028,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E32" s="79"/>
       <c r="F32" s="79"/>
@@ -5038,10 +5044,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E33" s="79"/>
       <c r="F33" s="79"/>
@@ -5054,10 +5060,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" s="77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34" s="79"/>
       <c r="F34" s="79"/>
@@ -5070,10 +5076,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E35" s="79"/>
       <c r="F35" s="79"/>
@@ -5086,10 +5092,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D36" s="77" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E36" s="79"/>
       <c r="F36" s="79"/>
@@ -5102,10 +5108,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37" s="77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E37" s="79"/>
       <c r="F37" s="79"/>
@@ -5118,10 +5124,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="79"/>
       <c r="F38" s="79"/>
@@ -5134,10 +5140,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" s="77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E39" s="79"/>
       <c r="F39" s="79"/>
@@ -5158,16 +5164,16 @@
         <v>2</v>
       </c>
       <c r="C41" s="77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F41" s="77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -5178,13 +5184,13 @@
         <v>2</v>
       </c>
       <c r="C42" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F42" s="79"/>
     </row>
@@ -5196,13 +5202,13 @@
         <v>2</v>
       </c>
       <c r="C43" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D43" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E43" s="77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" s="79"/>
     </row>
@@ -5214,10 +5220,10 @@
         <v>2</v>
       </c>
       <c r="C44" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="77" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E44" s="79"/>
       <c r="F44" s="79"/>
@@ -5230,10 +5236,10 @@
         <v>2</v>
       </c>
       <c r="C45" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" s="77" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E45" s="79"/>
       <c r="F45" s="79"/>
@@ -5246,10 +5252,10 @@
         <v>2</v>
       </c>
       <c r="C46" s="79" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="77" t="s">
         <v>90</v>
-      </c>
-      <c r="D46" s="77" t="s">
-        <v>91</v>
       </c>
       <c r="E46" s="79"/>
       <c r="F46" s="79"/>
@@ -5262,10 +5268,10 @@
         <v>2</v>
       </c>
       <c r="C47" s="79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E47" s="79"/>
       <c r="F47" s="79"/>
@@ -5284,7 +5290,7 @@
       </c>
       <c r="B49" s="143"/>
       <c r="C49" s="144" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D49" s="145"/>
       <c r="E49" s="145"/>
@@ -5298,16 +5304,16 @@
         <v>1</v>
       </c>
       <c r="C50" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="E50" s="77" t="s">
-        <v>99</v>
-      </c>
       <c r="F50" s="77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="76.5">
@@ -5319,10 +5325,10 @@
       </c>
       <c r="C51" s="79"/>
       <c r="D51" s="77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E51" s="77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F51" s="79"/>
     </row>
@@ -5336,7 +5342,7 @@
       <c r="C52" s="79"/>
       <c r="D52" s="79"/>
       <c r="E52" s="77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F52" s="79"/>
     </row>
@@ -5350,7 +5356,7 @@
       <c r="C53" s="79"/>
       <c r="D53" s="79"/>
       <c r="E53" s="77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F53" s="79"/>
     </row>
@@ -5364,7 +5370,7 @@
       <c r="C54" s="79"/>
       <c r="D54" s="79"/>
       <c r="E54" s="77" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F54" s="79"/>
     </row>
@@ -5384,16 +5390,16 @@
         <v>2</v>
       </c>
       <c r="C56" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D56" s="77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E56" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="51">
@@ -5405,10 +5411,10 @@
       </c>
       <c r="C57" s="79"/>
       <c r="D57" s="77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E57" s="77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F57" s="79"/>
     </row>
@@ -5421,10 +5427,10 @@
       </c>
       <c r="C58" s="79"/>
       <c r="D58" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E58" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F58" s="79"/>
     </row>
@@ -5444,16 +5450,16 @@
         <v>3</v>
       </c>
       <c r="C60" s="77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E60" s="77" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F60" s="77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -5465,13 +5471,13 @@
       </c>
       <c r="C61" s="79"/>
       <c r="D61" s="77" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E61" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" s="77" t="s">
         <v>121</v>
-      </c>
-      <c r="F61" s="77" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="58.5" customHeight="1">
@@ -5483,11 +5489,11 @@
       </c>
       <c r="C62" s="79"/>
       <c r="D62" s="77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E62" s="79"/>
       <c r="F62" s="77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="39.950000000000003" customHeight="1">
@@ -5499,7 +5505,7 @@
       </c>
       <c r="C63" s="79"/>
       <c r="D63" s="77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E63" s="79"/>
       <c r="F63" s="79"/>
@@ -5513,7 +5519,7 @@
       </c>
       <c r="C64" s="79"/>
       <c r="D64" s="77" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E64" s="79"/>
       <c r="F64" s="79"/>
@@ -5527,7 +5533,7 @@
       </c>
       <c r="C65" s="79"/>
       <c r="D65" s="77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E65" s="79"/>
       <c r="F65" s="79"/>
@@ -5541,7 +5547,7 @@
       </c>
       <c r="C66" s="79"/>
       <c r="D66" s="77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E66" s="79"/>
       <c r="F66" s="79"/>
@@ -5555,7 +5561,7 @@
       </c>
       <c r="C67" s="79"/>
       <c r="D67" s="77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E67" s="79"/>
       <c r="F67" s="79"/>
@@ -5569,7 +5575,7 @@
       </c>
       <c r="C68" s="79"/>
       <c r="D68" s="77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E68" s="79"/>
       <c r="F68" s="79"/>
@@ -5583,7 +5589,7 @@
       </c>
       <c r="C69" s="79"/>
       <c r="D69" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E69" s="79"/>
       <c r="F69" s="79"/>
@@ -5616,7 +5622,7 @@
       <pane xSplit="6" ySplit="12" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -5638,296 +5644,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="201"/>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
-      <c r="N1" s="201"/>
-      <c r="O1" s="201"/>
-      <c r="P1" s="201"/>
-      <c r="Q1" s="201"/>
-      <c r="R1" s="201"/>
-      <c r="S1" s="201"/>
-      <c r="T1" s="201"/>
-      <c r="U1" s="201"/>
-      <c r="V1" s="201"/>
-      <c r="W1" s="201"/>
-      <c r="X1" s="201"/>
-      <c r="Y1" s="201"/>
-      <c r="Z1" s="201"/>
-      <c r="AA1" s="201"/>
-      <c r="AB1" s="201"/>
-      <c r="AC1" s="201"/>
-      <c r="AD1" s="201"/>
-      <c r="AE1" s="201"/>
-      <c r="AF1" s="201"/>
-      <c r="AG1" s="201"/>
-      <c r="AH1" s="201"/>
-      <c r="AI1" s="201"/>
-      <c r="AJ1" s="201"/>
-      <c r="AK1" s="201"/>
-      <c r="AL1" s="201"/>
-      <c r="AM1" s="201"/>
-      <c r="AN1" s="201"/>
-      <c r="AO1" s="201"/>
-      <c r="AP1" s="201"/>
-      <c r="AQ1" s="201"/>
-      <c r="AR1" s="201"/>
-      <c r="AS1" s="201"/>
-      <c r="AT1" s="201"/>
-      <c r="AU1" s="201"/>
-      <c r="AV1" s="201"/>
-      <c r="AW1" s="201"/>
-      <c r="AX1" s="201"/>
-      <c r="AY1" s="201"/>
-      <c r="AZ1" s="201"/>
-      <c r="BA1" s="201"/>
-      <c r="BB1" s="201"/>
-      <c r="BC1" s="201"/>
-      <c r="BD1" s="201"/>
-      <c r="BE1" s="201"/>
-      <c r="BF1" s="201"/>
-      <c r="BG1" s="201"/>
-      <c r="BH1" s="201"/>
-      <c r="BI1" s="201"/>
-      <c r="BJ1" s="201"/>
-      <c r="BK1" s="201"/>
-      <c r="BL1" s="201"/>
-      <c r="BM1" s="201"/>
-      <c r="BN1" s="201"/>
-      <c r="BO1" s="201"/>
-      <c r="BP1" s="201"/>
-      <c r="BQ1" s="201"/>
-      <c r="BR1" s="201"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
+      <c r="N1" s="206"/>
+      <c r="O1" s="206"/>
+      <c r="P1" s="206"/>
+      <c r="Q1" s="206"/>
+      <c r="R1" s="206"/>
+      <c r="S1" s="206"/>
+      <c r="T1" s="206"/>
+      <c r="U1" s="206"/>
+      <c r="V1" s="206"/>
+      <c r="W1" s="206"/>
+      <c r="X1" s="206"/>
+      <c r="Y1" s="206"/>
+      <c r="Z1" s="206"/>
+      <c r="AA1" s="206"/>
+      <c r="AB1" s="206"/>
+      <c r="AC1" s="206"/>
+      <c r="AD1" s="206"/>
+      <c r="AE1" s="206"/>
+      <c r="AF1" s="206"/>
+      <c r="AG1" s="206"/>
+      <c r="AH1" s="206"/>
+      <c r="AI1" s="206"/>
+      <c r="AJ1" s="206"/>
+      <c r="AK1" s="206"/>
+      <c r="AL1" s="206"/>
+      <c r="AM1" s="206"/>
+      <c r="AN1" s="206"/>
+      <c r="AO1" s="206"/>
+      <c r="AP1" s="206"/>
+      <c r="AQ1" s="206"/>
+      <c r="AR1" s="206"/>
+      <c r="AS1" s="206"/>
+      <c r="AT1" s="206"/>
+      <c r="AU1" s="206"/>
+      <c r="AV1" s="206"/>
+      <c r="AW1" s="206"/>
+      <c r="AX1" s="206"/>
+      <c r="AY1" s="206"/>
+      <c r="AZ1" s="206"/>
+      <c r="BA1" s="206"/>
+      <c r="BB1" s="206"/>
+      <c r="BC1" s="206"/>
+      <c r="BD1" s="206"/>
+      <c r="BE1" s="206"/>
+      <c r="BF1" s="206"/>
+      <c r="BG1" s="206"/>
+      <c r="BH1" s="206"/>
+      <c r="BI1" s="206"/>
+      <c r="BJ1" s="206"/>
+      <c r="BK1" s="206"/>
+      <c r="BL1" s="206"/>
+      <c r="BM1" s="206"/>
+      <c r="BN1" s="206"/>
+      <c r="BO1" s="206"/>
+      <c r="BP1" s="206"/>
+      <c r="BQ1" s="206"/>
+      <c r="BR1" s="206"/>
     </row>
     <row r="2" spans="1:70" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="202" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="201"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="202"/>
-      <c r="R2" s="202"/>
-      <c r="S2" s="202"/>
-      <c r="T2" s="202"/>
-      <c r="U2" s="202"/>
-      <c r="V2" s="202"/>
-      <c r="W2" s="202"/>
-      <c r="X2" s="202"/>
-      <c r="Y2" s="202"/>
-      <c r="Z2" s="202"/>
-      <c r="AA2" s="202"/>
-      <c r="AB2" s="202"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="202"/>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="202"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="202"/>
-      <c r="AI2" s="202"/>
-      <c r="AJ2" s="202"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="202"/>
-      <c r="AM2" s="202"/>
-      <c r="AN2" s="202"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="202"/>
-      <c r="AQ2" s="202"/>
-      <c r="AR2" s="202"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="202"/>
-      <c r="AU2" s="202"/>
-      <c r="AV2" s="202"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="202"/>
-      <c r="AY2" s="202"/>
-      <c r="AZ2" s="202"/>
-      <c r="BA2" s="202"/>
-      <c r="BB2" s="202"/>
-      <c r="BC2" s="202"/>
-      <c r="BD2" s="202"/>
-      <c r="BE2" s="202"/>
-      <c r="BF2" s="202"/>
-      <c r="BG2" s="202"/>
-      <c r="BH2" s="202"/>
-      <c r="BI2" s="202"/>
-      <c r="BJ2" s="202"/>
-      <c r="BK2" s="202"/>
-      <c r="BL2" s="202"/>
-      <c r="BM2" s="202"/>
-      <c r="BN2" s="202"/>
-      <c r="BO2" s="202"/>
-      <c r="BP2" s="202"/>
-      <c r="BQ2" s="202"/>
-      <c r="BR2" s="203"/>
+      <c r="A2" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="206"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
+      <c r="Q2" s="207"/>
+      <c r="R2" s="207"/>
+      <c r="S2" s="207"/>
+      <c r="T2" s="207"/>
+      <c r="U2" s="207"/>
+      <c r="V2" s="207"/>
+      <c r="W2" s="207"/>
+      <c r="X2" s="207"/>
+      <c r="Y2" s="207"/>
+      <c r="Z2" s="207"/>
+      <c r="AA2" s="207"/>
+      <c r="AB2" s="207"/>
+      <c r="AC2" s="207"/>
+      <c r="AD2" s="207"/>
+      <c r="AE2" s="207"/>
+      <c r="AF2" s="207"/>
+      <c r="AG2" s="207"/>
+      <c r="AH2" s="207"/>
+      <c r="AI2" s="207"/>
+      <c r="AJ2" s="207"/>
+      <c r="AK2" s="207"/>
+      <c r="AL2" s="207"/>
+      <c r="AM2" s="207"/>
+      <c r="AN2" s="207"/>
+      <c r="AO2" s="207"/>
+      <c r="AP2" s="207"/>
+      <c r="AQ2" s="207"/>
+      <c r="AR2" s="207"/>
+      <c r="AS2" s="207"/>
+      <c r="AT2" s="207"/>
+      <c r="AU2" s="207"/>
+      <c r="AV2" s="207"/>
+      <c r="AW2" s="207"/>
+      <c r="AX2" s="207"/>
+      <c r="AY2" s="207"/>
+      <c r="AZ2" s="207"/>
+      <c r="BA2" s="207"/>
+      <c r="BB2" s="207"/>
+      <c r="BC2" s="207"/>
+      <c r="BD2" s="207"/>
+      <c r="BE2" s="207"/>
+      <c r="BF2" s="207"/>
+      <c r="BG2" s="207"/>
+      <c r="BH2" s="207"/>
+      <c r="BI2" s="207"/>
+      <c r="BJ2" s="207"/>
+      <c r="BK2" s="207"/>
+      <c r="BL2" s="207"/>
+      <c r="BM2" s="207"/>
+      <c r="BN2" s="207"/>
+      <c r="BO2" s="207"/>
+      <c r="BP2" s="207"/>
+      <c r="BQ2" s="207"/>
+      <c r="BR2" s="208"/>
     </row>
     <row r="3" spans="1:70" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="201"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="202"/>
-      <c r="Q3" s="202"/>
-      <c r="R3" s="202"/>
-      <c r="S3" s="202"/>
-      <c r="T3" s="202"/>
-      <c r="U3" s="202"/>
-      <c r="V3" s="202"/>
-      <c r="W3" s="202"/>
-      <c r="X3" s="202"/>
-      <c r="Y3" s="202"/>
-      <c r="Z3" s="202"/>
-      <c r="AA3" s="202"/>
-      <c r="AB3" s="202"/>
-      <c r="AC3" s="202"/>
-      <c r="AD3" s="202"/>
-      <c r="AE3" s="202"/>
-      <c r="AF3" s="202"/>
-      <c r="AG3" s="202"/>
-      <c r="AH3" s="202"/>
-      <c r="AI3" s="202"/>
-      <c r="AJ3" s="202"/>
-      <c r="AK3" s="202"/>
-      <c r="AL3" s="202"/>
-      <c r="AM3" s="202"/>
-      <c r="AN3" s="202"/>
-      <c r="AO3" s="202"/>
-      <c r="AP3" s="202"/>
-      <c r="AQ3" s="202"/>
-      <c r="AR3" s="202"/>
-      <c r="AS3" s="202"/>
-      <c r="AT3" s="202"/>
-      <c r="AU3" s="202"/>
-      <c r="AV3" s="202"/>
-      <c r="AW3" s="202"/>
-      <c r="AX3" s="202"/>
-      <c r="AY3" s="202"/>
-      <c r="AZ3" s="202"/>
-      <c r="BA3" s="202"/>
-      <c r="BB3" s="202"/>
-      <c r="BC3" s="202"/>
-      <c r="BD3" s="202"/>
-      <c r="BE3" s="202"/>
-      <c r="BF3" s="202"/>
-      <c r="BG3" s="202"/>
-      <c r="BH3" s="202"/>
-      <c r="BI3" s="202"/>
-      <c r="BJ3" s="202"/>
-      <c r="BK3" s="202"/>
-      <c r="BL3" s="202"/>
-      <c r="BM3" s="202"/>
-      <c r="BN3" s="202"/>
-      <c r="BO3" s="202"/>
-      <c r="BP3" s="202"/>
-      <c r="BQ3" s="202"/>
-      <c r="BR3" s="203"/>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="206"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="207"/>
+      <c r="N3" s="207"/>
+      <c r="O3" s="207"/>
+      <c r="P3" s="207"/>
+      <c r="Q3" s="207"/>
+      <c r="R3" s="207"/>
+      <c r="S3" s="207"/>
+      <c r="T3" s="207"/>
+      <c r="U3" s="207"/>
+      <c r="V3" s="207"/>
+      <c r="W3" s="207"/>
+      <c r="X3" s="207"/>
+      <c r="Y3" s="207"/>
+      <c r="Z3" s="207"/>
+      <c r="AA3" s="207"/>
+      <c r="AB3" s="207"/>
+      <c r="AC3" s="207"/>
+      <c r="AD3" s="207"/>
+      <c r="AE3" s="207"/>
+      <c r="AF3" s="207"/>
+      <c r="AG3" s="207"/>
+      <c r="AH3" s="207"/>
+      <c r="AI3" s="207"/>
+      <c r="AJ3" s="207"/>
+      <c r="AK3" s="207"/>
+      <c r="AL3" s="207"/>
+      <c r="AM3" s="207"/>
+      <c r="AN3" s="207"/>
+      <c r="AO3" s="207"/>
+      <c r="AP3" s="207"/>
+      <c r="AQ3" s="207"/>
+      <c r="AR3" s="207"/>
+      <c r="AS3" s="207"/>
+      <c r="AT3" s="207"/>
+      <c r="AU3" s="207"/>
+      <c r="AV3" s="207"/>
+      <c r="AW3" s="207"/>
+      <c r="AX3" s="207"/>
+      <c r="AY3" s="207"/>
+      <c r="AZ3" s="207"/>
+      <c r="BA3" s="207"/>
+      <c r="BB3" s="207"/>
+      <c r="BC3" s="207"/>
+      <c r="BD3" s="207"/>
+      <c r="BE3" s="207"/>
+      <c r="BF3" s="207"/>
+      <c r="BG3" s="207"/>
+      <c r="BH3" s="207"/>
+      <c r="BI3" s="207"/>
+      <c r="BJ3" s="207"/>
+      <c r="BK3" s="207"/>
+      <c r="BL3" s="207"/>
+      <c r="BM3" s="207"/>
+      <c r="BN3" s="207"/>
+      <c r="BO3" s="207"/>
+      <c r="BP3" s="207"/>
+      <c r="BQ3" s="207"/>
+      <c r="BR3" s="208"/>
     </row>
     <row r="4" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A4" s="204"/>
-      <c r="B4" s="204"/>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
-      <c r="K4" s="204"/>
-      <c r="L4" s="204"/>
-      <c r="M4" s="204"/>
-      <c r="N4" s="204"/>
-      <c r="O4" s="204"/>
-      <c r="P4" s="204"/>
-      <c r="Q4" s="204"/>
-      <c r="R4" s="204"/>
-      <c r="S4" s="204"/>
-      <c r="T4" s="204"/>
-      <c r="U4" s="204"/>
-      <c r="V4" s="204"/>
-      <c r="W4" s="204"/>
-      <c r="X4" s="204"/>
-      <c r="Y4" s="204"/>
-      <c r="Z4" s="204"/>
-      <c r="AA4" s="204"/>
-      <c r="AB4" s="204"/>
-      <c r="AC4" s="204"/>
-      <c r="AD4" s="204"/>
-      <c r="AE4" s="204"/>
-      <c r="AF4" s="204"/>
-      <c r="AG4" s="204"/>
-      <c r="AH4" s="204"/>
-      <c r="AI4" s="204"/>
-      <c r="AJ4" s="204"/>
-      <c r="AK4" s="204"/>
-      <c r="AL4" s="204"/>
-      <c r="AM4" s="204"/>
-      <c r="AN4" s="204"/>
-      <c r="AO4" s="204"/>
-      <c r="AP4" s="204"/>
-      <c r="AQ4" s="204"/>
-      <c r="AR4" s="204"/>
-      <c r="AS4" s="204"/>
-      <c r="AT4" s="204"/>
-      <c r="AU4" s="204"/>
-      <c r="AV4" s="204"/>
-      <c r="AW4" s="204"/>
-      <c r="AX4" s="204"/>
-      <c r="AY4" s="204"/>
-      <c r="AZ4" s="204"/>
-      <c r="BA4" s="204"/>
-      <c r="BB4" s="204"/>
-      <c r="BC4" s="204"/>
-      <c r="BD4" s="204"/>
-      <c r="BE4" s="204"/>
-      <c r="BF4" s="204"/>
-      <c r="BG4" s="204"/>
-      <c r="BH4" s="204"/>
-      <c r="BI4" s="204"/>
-      <c r="BJ4" s="204"/>
-      <c r="BK4" s="204"/>
-      <c r="BL4" s="204"/>
-      <c r="BM4" s="204"/>
-      <c r="BN4" s="204"/>
-      <c r="BO4" s="204"/>
-      <c r="BP4" s="204"/>
-      <c r="BQ4" s="204"/>
-      <c r="BR4" s="205"/>
+      <c r="A4" s="209"/>
+      <c r="B4" s="209"/>
+      <c r="C4" s="209"/>
+      <c r="D4" s="209"/>
+      <c r="E4" s="209"/>
+      <c r="F4" s="209"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="209"/>
+      <c r="I4" s="209"/>
+      <c r="J4" s="209"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="209"/>
+      <c r="M4" s="209"/>
+      <c r="N4" s="209"/>
+      <c r="O4" s="209"/>
+      <c r="P4" s="209"/>
+      <c r="Q4" s="209"/>
+      <c r="R4" s="209"/>
+      <c r="S4" s="209"/>
+      <c r="T4" s="209"/>
+      <c r="U4" s="209"/>
+      <c r="V4" s="209"/>
+      <c r="W4" s="209"/>
+      <c r="X4" s="209"/>
+      <c r="Y4" s="209"/>
+      <c r="Z4" s="209"/>
+      <c r="AA4" s="209"/>
+      <c r="AB4" s="209"/>
+      <c r="AC4" s="209"/>
+      <c r="AD4" s="209"/>
+      <c r="AE4" s="209"/>
+      <c r="AF4" s="209"/>
+      <c r="AG4" s="209"/>
+      <c r="AH4" s="209"/>
+      <c r="AI4" s="209"/>
+      <c r="AJ4" s="209"/>
+      <c r="AK4" s="209"/>
+      <c r="AL4" s="209"/>
+      <c r="AM4" s="209"/>
+      <c r="AN4" s="209"/>
+      <c r="AO4" s="209"/>
+      <c r="AP4" s="209"/>
+      <c r="AQ4" s="209"/>
+      <c r="AR4" s="209"/>
+      <c r="AS4" s="209"/>
+      <c r="AT4" s="209"/>
+      <c r="AU4" s="209"/>
+      <c r="AV4" s="209"/>
+      <c r="AW4" s="209"/>
+      <c r="AX4" s="209"/>
+      <c r="AY4" s="209"/>
+      <c r="AZ4" s="209"/>
+      <c r="BA4" s="209"/>
+      <c r="BB4" s="209"/>
+      <c r="BC4" s="209"/>
+      <c r="BD4" s="209"/>
+      <c r="BE4" s="209"/>
+      <c r="BF4" s="209"/>
+      <c r="BG4" s="209"/>
+      <c r="BH4" s="209"/>
+      <c r="BI4" s="209"/>
+      <c r="BJ4" s="209"/>
+      <c r="BK4" s="209"/>
+      <c r="BL4" s="209"/>
+      <c r="BM4" s="209"/>
+      <c r="BN4" s="209"/>
+      <c r="BO4" s="209"/>
+      <c r="BP4" s="209"/>
+      <c r="BQ4" s="209"/>
+      <c r="BR4" s="210"/>
     </row>
     <row r="5" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickTop="1">
       <c r="A5" s="113"/>
@@ -6039,195 +6045,195 @@
     </row>
     <row r="8" spans="1:70" ht="17.25" customHeight="1">
       <c r="B8" s="125" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="126"/>
-      <c r="D8" s="215">
+      <c r="D8" s="205">
         <v>45486</v>
       </c>
-      <c r="E8" s="215"/>
-      <c r="F8" s="215"/>
+      <c r="E8" s="205"/>
+      <c r="F8" s="205"/>
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="K8" s="138" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="O8" s="210" t="str">
+      <c r="O8" s="202" t="str">
         <f>"Semana "&amp;(O10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 1</v>
       </c>
-      <c r="P8" s="211"/>
-      <c r="Q8" s="211"/>
-      <c r="R8" s="211"/>
-      <c r="S8" s="211"/>
-      <c r="T8" s="211"/>
-      <c r="U8" s="212"/>
-      <c r="V8" s="210" t="str">
+      <c r="P8" s="203"/>
+      <c r="Q8" s="203"/>
+      <c r="R8" s="203"/>
+      <c r="S8" s="203"/>
+      <c r="T8" s="203"/>
+      <c r="U8" s="204"/>
+      <c r="V8" s="202" t="str">
         <f>"Semana "&amp;(V10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 2</v>
       </c>
-      <c r="W8" s="211"/>
-      <c r="X8" s="211"/>
-      <c r="Y8" s="211"/>
-      <c r="Z8" s="211"/>
-      <c r="AA8" s="211"/>
-      <c r="AB8" s="212"/>
-      <c r="AC8" s="210" t="str">
+      <c r="W8" s="203"/>
+      <c r="X8" s="203"/>
+      <c r="Y8" s="203"/>
+      <c r="Z8" s="203"/>
+      <c r="AA8" s="203"/>
+      <c r="AB8" s="204"/>
+      <c r="AC8" s="202" t="str">
         <f>"Semana "&amp;(AC10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 3</v>
       </c>
-      <c r="AD8" s="211"/>
-      <c r="AE8" s="211"/>
-      <c r="AF8" s="211"/>
-      <c r="AG8" s="211"/>
-      <c r="AH8" s="211"/>
-      <c r="AI8" s="212"/>
-      <c r="AJ8" s="210" t="str">
+      <c r="AD8" s="203"/>
+      <c r="AE8" s="203"/>
+      <c r="AF8" s="203"/>
+      <c r="AG8" s="203"/>
+      <c r="AH8" s="203"/>
+      <c r="AI8" s="204"/>
+      <c r="AJ8" s="202" t="str">
         <f>"Semana "&amp;(AJ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 4</v>
       </c>
-      <c r="AK8" s="211"/>
-      <c r="AL8" s="211"/>
-      <c r="AM8" s="211"/>
-      <c r="AN8" s="211"/>
-      <c r="AO8" s="211"/>
-      <c r="AP8" s="212"/>
-      <c r="AQ8" s="210" t="str">
+      <c r="AK8" s="203"/>
+      <c r="AL8" s="203"/>
+      <c r="AM8" s="203"/>
+      <c r="AN8" s="203"/>
+      <c r="AO8" s="203"/>
+      <c r="AP8" s="204"/>
+      <c r="AQ8" s="202" t="str">
         <f>"Semana "&amp;(AQ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 5</v>
       </c>
-      <c r="AR8" s="211"/>
-      <c r="AS8" s="211"/>
-      <c r="AT8" s="211"/>
-      <c r="AU8" s="211"/>
-      <c r="AV8" s="211"/>
-      <c r="AW8" s="212"/>
-      <c r="AX8" s="210" t="str">
+      <c r="AR8" s="203"/>
+      <c r="AS8" s="203"/>
+      <c r="AT8" s="203"/>
+      <c r="AU8" s="203"/>
+      <c r="AV8" s="203"/>
+      <c r="AW8" s="204"/>
+      <c r="AX8" s="202" t="str">
         <f>"Semana "&amp;(AX10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 6</v>
       </c>
-      <c r="AY8" s="211"/>
-      <c r="AZ8" s="211"/>
-      <c r="BA8" s="211"/>
-      <c r="BB8" s="211"/>
-      <c r="BC8" s="211"/>
-      <c r="BD8" s="212"/>
-      <c r="BE8" s="210" t="str">
+      <c r="AY8" s="203"/>
+      <c r="AZ8" s="203"/>
+      <c r="BA8" s="203"/>
+      <c r="BB8" s="203"/>
+      <c r="BC8" s="203"/>
+      <c r="BD8" s="204"/>
+      <c r="BE8" s="202" t="str">
         <f>"Semana "&amp;(BE10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 7</v>
       </c>
-      <c r="BF8" s="211"/>
-      <c r="BG8" s="211"/>
-      <c r="BH8" s="211"/>
-      <c r="BI8" s="211"/>
-      <c r="BJ8" s="211"/>
-      <c r="BK8" s="212"/>
-      <c r="BL8" s="210" t="str">
+      <c r="BF8" s="203"/>
+      <c r="BG8" s="203"/>
+      <c r="BH8" s="203"/>
+      <c r="BI8" s="203"/>
+      <c r="BJ8" s="203"/>
+      <c r="BK8" s="204"/>
+      <c r="BL8" s="202" t="str">
         <f>"Semana "&amp;(BL10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 8</v>
       </c>
-      <c r="BM8" s="211"/>
-      <c r="BN8" s="211"/>
-      <c r="BO8" s="211"/>
-      <c r="BP8" s="211"/>
-      <c r="BQ8" s="211"/>
-      <c r="BR8" s="213"/>
+      <c r="BM8" s="203"/>
+      <c r="BN8" s="203"/>
+      <c r="BO8" s="203"/>
+      <c r="BP8" s="203"/>
+      <c r="BQ8" s="203"/>
+      <c r="BR8" s="215"/>
     </row>
     <row r="9" spans="1:70" ht="17.25" customHeight="1">
       <c r="B9" s="125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="126"/>
-      <c r="D9" s="214" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="214"/>
-      <c r="F9" s="214"/>
+      <c r="D9" s="201" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="O9" s="206">
+      <c r="O9" s="211">
         <f>O10</f>
         <v>45481</v>
       </c>
-      <c r="P9" s="207"/>
-      <c r="Q9" s="207"/>
-      <c r="R9" s="207"/>
-      <c r="S9" s="207"/>
-      <c r="T9" s="207"/>
-      <c r="U9" s="208"/>
-      <c r="V9" s="206">
+      <c r="P9" s="212"/>
+      <c r="Q9" s="212"/>
+      <c r="R9" s="212"/>
+      <c r="S9" s="212"/>
+      <c r="T9" s="212"/>
+      <c r="U9" s="213"/>
+      <c r="V9" s="211">
         <f>V10</f>
         <v>45488</v>
       </c>
-      <c r="W9" s="207"/>
-      <c r="X9" s="207"/>
-      <c r="Y9" s="207"/>
-      <c r="Z9" s="207"/>
-      <c r="AA9" s="207"/>
-      <c r="AB9" s="208"/>
-      <c r="AC9" s="206">
+      <c r="W9" s="212"/>
+      <c r="X9" s="212"/>
+      <c r="Y9" s="212"/>
+      <c r="Z9" s="212"/>
+      <c r="AA9" s="212"/>
+      <c r="AB9" s="213"/>
+      <c r="AC9" s="211">
         <f>AC10</f>
         <v>45495</v>
       </c>
-      <c r="AD9" s="207"/>
-      <c r="AE9" s="207"/>
-      <c r="AF9" s="207"/>
-      <c r="AG9" s="207"/>
-      <c r="AH9" s="207"/>
-      <c r="AI9" s="208"/>
-      <c r="AJ9" s="206">
+      <c r="AD9" s="212"/>
+      <c r="AE9" s="212"/>
+      <c r="AF9" s="212"/>
+      <c r="AG9" s="212"/>
+      <c r="AH9" s="212"/>
+      <c r="AI9" s="213"/>
+      <c r="AJ9" s="211">
         <f>AJ10</f>
         <v>45502</v>
       </c>
-      <c r="AK9" s="207"/>
-      <c r="AL9" s="207"/>
-      <c r="AM9" s="207"/>
-      <c r="AN9" s="207"/>
-      <c r="AO9" s="207"/>
-      <c r="AP9" s="208"/>
-      <c r="AQ9" s="206">
+      <c r="AK9" s="212"/>
+      <c r="AL9" s="212"/>
+      <c r="AM9" s="212"/>
+      <c r="AN9" s="212"/>
+      <c r="AO9" s="212"/>
+      <c r="AP9" s="213"/>
+      <c r="AQ9" s="211">
         <f>AQ10</f>
         <v>45509</v>
       </c>
-      <c r="AR9" s="207"/>
-      <c r="AS9" s="207"/>
-      <c r="AT9" s="207"/>
-      <c r="AU9" s="207"/>
-      <c r="AV9" s="207"/>
-      <c r="AW9" s="208"/>
-      <c r="AX9" s="206">
+      <c r="AR9" s="212"/>
+      <c r="AS9" s="212"/>
+      <c r="AT9" s="212"/>
+      <c r="AU9" s="212"/>
+      <c r="AV9" s="212"/>
+      <c r="AW9" s="213"/>
+      <c r="AX9" s="211">
         <f>AX10</f>
         <v>45516</v>
       </c>
-      <c r="AY9" s="207"/>
-      <c r="AZ9" s="207"/>
-      <c r="BA9" s="207"/>
-      <c r="BB9" s="207"/>
-      <c r="BC9" s="207"/>
-      <c r="BD9" s="208"/>
-      <c r="BE9" s="206">
+      <c r="AY9" s="212"/>
+      <c r="AZ9" s="212"/>
+      <c r="BA9" s="212"/>
+      <c r="BB9" s="212"/>
+      <c r="BC9" s="212"/>
+      <c r="BD9" s="213"/>
+      <c r="BE9" s="211">
         <f>BE10</f>
         <v>45523</v>
       </c>
-      <c r="BF9" s="207"/>
-      <c r="BG9" s="207"/>
-      <c r="BH9" s="207"/>
-      <c r="BI9" s="207"/>
-      <c r="BJ9" s="207"/>
-      <c r="BK9" s="208"/>
-      <c r="BL9" s="206">
+      <c r="BF9" s="212"/>
+      <c r="BG9" s="212"/>
+      <c r="BH9" s="212"/>
+      <c r="BI9" s="212"/>
+      <c r="BJ9" s="212"/>
+      <c r="BK9" s="213"/>
+      <c r="BL9" s="211">
         <f>BL10</f>
         <v>45530</v>
       </c>
-      <c r="BM9" s="207"/>
-      <c r="BN9" s="207"/>
-      <c r="BO9" s="207"/>
-      <c r="BP9" s="207"/>
-      <c r="BQ9" s="207"/>
-      <c r="BR9" s="209"/>
+      <c r="BM9" s="212"/>
+      <c r="BN9" s="212"/>
+      <c r="BO9" s="212"/>
+      <c r="BP9" s="212"/>
+      <c r="BQ9" s="212"/>
+      <c r="BR9" s="214"/>
     </row>
     <row r="10" spans="1:70">
       <c r="O10" s="33">
@@ -6457,43 +6463,43 @@
     </row>
     <row r="11" spans="1:70" s="167" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A11" s="162" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="162" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="162" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="162" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="162" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="162" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="162" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="161" t="s">
+      <c r="G11" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="161" t="s">
+      <c r="H11" s="161" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="161" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="162" t="s">
+      <c r="J11" s="162" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="162" t="s">
+      <c r="K11" s="161" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="161" t="s">
+      <c r="L11" s="161" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="161" t="s">
         <v>40</v>
-      </c>
-      <c r="L11" s="161" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="161" t="s">
-        <v>41</v>
       </c>
       <c r="N11" s="161"/>
       <c r="O11" s="163" t="str">
@@ -6727,16 +6733,16 @@
         <v>1</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="95"/>
       <c r="G12" s="95"/>
@@ -6816,10 +6822,10 @@
         <v>1.1</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" s="47">
         <v>220501092</v>
@@ -6828,7 +6834,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G13" s="90"/>
       <c r="H13" s="49"/>
@@ -6911,10 +6917,10 @@
         <v>1.2</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D14" s="47">
         <v>220501092</v>
@@ -6923,7 +6929,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" s="90"/>
       <c r="H14" s="49"/>
@@ -7006,10 +7012,10 @@
         <v>1.3</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D15" s="47">
         <v>220501092</v>
@@ -7018,7 +7024,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" s="90"/>
       <c r="H15" s="49"/>
@@ -7101,10 +7107,10 @@
         <v>1.4</v>
       </c>
       <c r="B16" s="81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" s="47">
         <v>220501092</v>
@@ -7113,7 +7119,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G16" s="90"/>
       <c r="H16" s="49"/>
@@ -7196,10 +7202,10 @@
         <v>1.5</v>
       </c>
       <c r="B17" s="81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="47">
         <v>220501092</v>
@@ -7208,7 +7214,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G17" s="90"/>
       <c r="H17" s="49"/>
@@ -7291,10 +7297,10 @@
         <v>1.6</v>
       </c>
       <c r="B18" s="77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18" s="47">
         <v>220501092</v>
@@ -7303,7 +7309,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G18" s="91"/>
       <c r="H18" s="85"/>
@@ -7386,10 +7392,10 @@
         <v>1.7</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="47">
         <v>220501092</v>
@@ -7398,7 +7404,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G19" s="90"/>
       <c r="H19" s="49"/>
@@ -7481,10 +7487,10 @@
         <v>1.8</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D20" s="47">
         <v>220501092</v>
@@ -7493,7 +7499,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G20" s="90"/>
       <c r="H20" s="49"/>
@@ -7576,10 +7582,10 @@
         <v>1.9</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C21" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21" s="47">
         <v>220501092</v>
@@ -7588,7 +7594,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G21" s="90"/>
       <c r="H21" s="49"/>
@@ -7671,10 +7677,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
@@ -7756,10 +7762,10 @@
         <v>2.1</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="47">
         <v>220501096</v>
@@ -7768,7 +7774,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G23" s="90"/>
       <c r="H23" s="49"/>
@@ -7851,10 +7857,10 @@
         <v>2.2</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D24" s="47">
         <v>220501113</v>
@@ -7863,7 +7869,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G24" s="90"/>
       <c r="H24" s="49"/>
@@ -7946,10 +7952,10 @@
         <v>2.3</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="47">
         <v>220501113</v>
@@ -7958,7 +7964,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G25" s="90"/>
       <c r="H25" s="49"/>
@@ -8041,10 +8047,10 @@
         <v>2.4</v>
       </c>
       <c r="B26" s="48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C26" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D26" s="47">
         <v>220501113</v>
@@ -8053,7 +8059,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G26" s="90"/>
       <c r="H26" s="49"/>
@@ -8136,10 +8142,10 @@
         <v>2.5</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" s="47">
         <v>220501113</v>
@@ -8148,7 +8154,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G27" s="90"/>
       <c r="H27" s="49"/>
@@ -8231,10 +8237,10 @@
         <v>2.6</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C28" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" s="47">
         <v>220501113</v>
@@ -8243,7 +8249,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G28" s="90"/>
       <c r="H28" s="49"/>
@@ -8326,10 +8332,10 @@
         <v>2.7</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C29" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D29" s="47">
         <v>220501113</v>
@@ -8338,7 +8344,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G29" s="90"/>
       <c r="H29" s="49"/>
@@ -8421,10 +8427,10 @@
         <v>2.8</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C30" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" s="47">
         <v>220501113</v>
@@ -8433,7 +8439,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G30" s="90"/>
       <c r="H30" s="49"/>
@@ -8516,10 +8522,10 @@
         <v>2.9</v>
       </c>
       <c r="B31" s="48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C31" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="47">
         <v>220501113</v>
@@ -8528,7 +8534,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="90"/>
       <c r="H31" s="49"/>
@@ -8611,10 +8617,10 @@
         <v>2.10</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C32" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D32" s="47">
         <v>220501113</v>
@@ -8623,7 +8629,7 @@
         <v>2</v>
       </c>
       <c r="F32" s="48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G32" s="90"/>
       <c r="H32" s="49"/>
@@ -8706,10 +8712,10 @@
         <v>2.11</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D33" s="47">
         <v>220501113</v>
@@ -8718,7 +8724,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G33" s="90"/>
       <c r="H33" s="49"/>
@@ -8801,10 +8807,10 @@
         <v>2.12</v>
       </c>
       <c r="B34" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="47">
         <v>220501113</v>
@@ -8813,7 +8819,7 @@
         <v>2</v>
       </c>
       <c r="F34" s="48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G34" s="90"/>
       <c r="H34" s="49"/>
@@ -8896,10 +8902,10 @@
         <v>2.13</v>
       </c>
       <c r="B35" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C35" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D35" s="47">
         <v>220501113</v>
@@ -8908,7 +8914,7 @@
         <v>2</v>
       </c>
       <c r="F35" s="48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G35" s="90"/>
       <c r="H35" s="49"/>
@@ -8991,10 +8997,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="58"/>
       <c r="E36" s="58"/>
@@ -9076,10 +9082,10 @@
         <v>3.1</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C37" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D37" s="47">
         <v>220501096</v>
@@ -9088,7 +9094,7 @@
         <v>2</v>
       </c>
       <c r="F37" s="48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G37" s="90"/>
       <c r="H37" s="49"/>
@@ -9171,10 +9177,10 @@
         <v>3.2</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D38" s="47">
         <v>220501096</v>
@@ -9183,7 +9189,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G38" s="90"/>
       <c r="H38" s="49"/>
@@ -9266,10 +9272,10 @@
         <v>3.3</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C39" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="47">
         <v>220501096</v>
@@ -9278,7 +9284,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G39" s="90"/>
       <c r="H39" s="49"/>
@@ -9361,10 +9367,10 @@
         <v>3.4</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C40" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D40" s="47">
         <v>220501096</v>
@@ -9373,7 +9379,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G40" s="90"/>
       <c r="H40" s="49"/>
@@ -9456,10 +9462,10 @@
         <v>3.5</v>
       </c>
       <c r="B41" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C41" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D41" s="47">
         <v>220501096</v>
@@ -9468,7 +9474,7 @@
         <v>2</v>
       </c>
       <c r="F41" s="48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G41" s="90"/>
       <c r="H41" s="49"/>
@@ -9551,10 +9557,10 @@
         <v>3.6</v>
       </c>
       <c r="B42" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C42" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D42" s="47">
         <v>220501096</v>
@@ -9563,7 +9569,7 @@
         <v>3</v>
       </c>
       <c r="F42" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G42" s="90"/>
       <c r="H42" s="49"/>
@@ -9646,10 +9652,10 @@
         <v>3.7</v>
       </c>
       <c r="B43" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C43" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D43" s="47">
         <v>220501096</v>
@@ -9658,7 +9664,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G43" s="90"/>
       <c r="H43" s="49"/>
@@ -9741,10 +9747,10 @@
         <v>3.8</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C44" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D44" s="47">
         <v>220501096</v>
@@ -9753,7 +9759,7 @@
         <v>3</v>
       </c>
       <c r="F44" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G44" s="90"/>
       <c r="H44" s="49"/>
@@ -9836,10 +9842,10 @@
         <v>3.9</v>
       </c>
       <c r="B45" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C45" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D45" s="47">
         <v>220501096</v>
@@ -9848,7 +9854,7 @@
         <v>3</v>
       </c>
       <c r="F45" s="48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G45" s="90"/>
       <c r="H45" s="49"/>
@@ -9931,10 +9937,10 @@
         <v>3.10</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D46" s="47">
         <v>220501096</v>
@@ -9943,7 +9949,7 @@
         <v>3</v>
       </c>
       <c r="F46" s="48" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G46" s="90"/>
       <c r="H46" s="49"/>
@@ -10026,10 +10032,10 @@
         <v>4</v>
       </c>
       <c r="B47" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="58"/>
       <c r="E47" s="58"/>
@@ -10111,10 +10117,10 @@
         <v>4.1</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C48" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D48" s="47">
         <v>220501096</v>
@@ -10123,7 +10129,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G48" s="90"/>
       <c r="H48" s="49"/>
@@ -10206,10 +10212,10 @@
         <v>4.2</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C49" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D49" s="47">
         <v>220501096</v>
@@ -10218,7 +10224,7 @@
         <v>3</v>
       </c>
       <c r="F49" s="48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G49" s="90"/>
       <c r="H49" s="49"/>
@@ -10301,10 +10307,10 @@
         <v>4.3</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C50" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D50" s="47">
         <v>220501096</v>
@@ -10313,7 +10319,7 @@
         <v>3</v>
       </c>
       <c r="F50" s="48" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G50" s="90"/>
       <c r="H50" s="49"/>
@@ -10396,10 +10402,10 @@
         <v>4.4</v>
       </c>
       <c r="B51" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C51" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D51" s="47">
         <v>220501096</v>
@@ -10408,7 +10414,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G51" s="90"/>
       <c r="H51" s="49"/>
@@ -10491,10 +10497,10 @@
         <v>4.5</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C52" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D52" s="47">
         <v>220501096</v>
@@ -10503,7 +10509,7 @@
         <v>3</v>
       </c>
       <c r="F52" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G52" s="90"/>
       <c r="H52" s="49"/>
@@ -10586,10 +10592,10 @@
         <v>4.6</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C53" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D53" s="47">
         <v>220501096</v>
@@ -10598,7 +10604,7 @@
         <v>3</v>
       </c>
       <c r="F53" s="48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G53" s="90"/>
       <c r="H53" s="49"/>
@@ -10681,10 +10687,10 @@
         <v>4.7</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C54" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D54" s="47">
         <v>220501096</v>
@@ -10693,7 +10699,7 @@
         <v>3</v>
       </c>
       <c r="F54" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G54" s="90"/>
       <c r="H54" s="49"/>
@@ -10846,12 +10852,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A11:M54" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="22">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="O8:U8"/>
-    <mergeCell ref="V8:AB8"/>
-    <mergeCell ref="AC8:AI8"/>
-    <mergeCell ref="AJ8:AP8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="A1:BR1"/>
     <mergeCell ref="A2:BR2"/>
     <mergeCell ref="A3:BR3"/>
@@ -10868,6 +10868,12 @@
     <mergeCell ref="AC9:AI9"/>
     <mergeCell ref="AJ9:AP9"/>
     <mergeCell ref="AQ9:AW9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="O8:U8"/>
+    <mergeCell ref="V8:AB8"/>
+    <mergeCell ref="AC8:AI8"/>
+    <mergeCell ref="AJ8:AP8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="L12:L22 L36:L46">
     <cfRule type="dataBar" priority="117">
@@ -11152,59 +11158,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="201"/>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="202" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
+      <c r="A2" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="202" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="202"/>
+      <c r="A3" s="207" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="207"/>
+      <c r="N3" s="207"/>
+      <c r="O3" s="207"/>
+      <c r="P3" s="207"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11243,7 +11249,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -11252,59 +11258,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="201"/>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="202" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
+      <c r="A2" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="202" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="202"/>
+      <c r="A3" s="207" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="207"/>
+      <c r="N3" s="207"/>
+      <c r="O3" s="207"/>
+      <c r="P3" s="207"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11352,59 +11358,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="201"/>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="202" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
+      <c r="A2" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="202" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="202"/>
+      <c r="A3" s="207" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="207"/>
+      <c r="N3" s="207"/>
+      <c r="O3" s="207"/>
+      <c r="P3" s="207"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11443,7 +11449,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -11452,59 +11458,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="201"/>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
-      <c r="K1" s="201"/>
-      <c r="L1" s="201"/>
-      <c r="M1" s="201"/>
+      <c r="A1" s="206"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+      <c r="L1" s="206"/>
+      <c r="M1" s="206"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="202" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="202"/>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="202"/>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
+      <c r="A2" s="207" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="207"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="202" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="202"/>
-      <c r="I3" s="202"/>
-      <c r="J3" s="202"/>
-      <c r="K3" s="202"/>
-      <c r="L3" s="202"/>
-      <c r="M3" s="202"/>
-      <c r="N3" s="202"/>
-      <c r="O3" s="202"/>
-      <c r="P3" s="202"/>
+      <c r="A3" s="207" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="207"/>
+      <c r="N3" s="207"/>
+      <c r="O3" s="207"/>
+      <c r="P3" s="207"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>

</xml_diff>

<commit_message>
Se ajusto el cronograma
</commit_message>
<xml_diff>
--- a/assets/Trimestres/Trimestre_3/Cronograma TPS_2926378_V2.xlsx
+++ b/assets/Trimestres/Trimestre_3/Cronograma TPS_2926378_V2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F660B35-B272-4127-BF62-6BA4E2D49A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC70F6BA-623D-477D-A78C-F72758A23840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" xr2:uid="{2EF96F3D-4256-48DD-8CAA-143A5EBF2E06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="812" activeTab="2" xr2:uid="{2EF96F3D-4256-48DD-8CAA-143A5EBF2E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Cronograma de Actividades'!$A$11:$M$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TPS!$A$1:$F$8</definedName>
+    <definedName name="prevWBS" localSheetId="2">'Cronograma de Actividades'!$A1048576</definedName>
+    <definedName name="prevWBS" localSheetId="1">TPS!$A1048576</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Cronograma de Actividades'!$A$1:$BR$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja de Control'!$B$2:$F$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">TPS!$A$3:$F$8</definedName>
-    <definedName name="prevWBS" localSheetId="2">'Cronograma de Actividades'!$A1048576</definedName>
-    <definedName name="prevWBS" localSheetId="1">TPS!$A1048576</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Cronograma de Actividades'!$1:$7</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">TPS!#REF!</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -32,11 +32,24 @@
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="247">
   <si>
     <t>Cronograma de Actividades</t>
   </si>
@@ -775,6 +788,24 @@
   </si>
   <si>
     <t>10/04/2024</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Ya</t>
+  </si>
+  <si>
+    <t>Daniel y Jenni</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Brayan</t>
   </si>
 </sst>
 </file>
@@ -2813,6 +2844,44 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2838,7 +2907,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2848,9 +2916,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2868,90 +2933,56 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="79" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="21" fillId="0" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="79" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
@@ -3998,11 +4029,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:P82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="2" customWidth="1"/>
@@ -4021,91 +4052,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="182" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="182"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="169"/>
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
+      <c r="B5" s="183"/>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="3"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="197"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="170"/>
+      <c r="F8" s="170"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="178" t="s">
+      <c r="C11" s="191" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="179"/>
-      <c r="E11" s="179"/>
-      <c r="F11" s="180"/>
+      <c r="D11" s="192"/>
+      <c r="E11" s="192"/>
+      <c r="F11" s="193"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="181" t="s">
+      <c r="C12" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="D12" s="182"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="183"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="195"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="181" t="s">
+      <c r="C13" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="182"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="183"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="196"/>
+      <c r="F13" s="195"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="181" t="s">
+      <c r="C14" s="168" t="s">
         <v>235</v>
       </c>
-      <c r="D14" s="196"/>
+      <c r="D14" s="169"/>
       <c r="E14" s="28" t="s">
         <v>7</v>
       </c>
@@ -4117,10 +4148,10 @@
       <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="185" t="s">
+      <c r="C15" s="197" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="186"/>
+      <c r="D15" s="198"/>
       <c r="E15" s="29" t="s">
         <v>9</v>
       </c>
@@ -4132,10 +4163,10 @@
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="187" t="s">
+      <c r="C16" s="199" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="188"/>
+      <c r="D16" s="200"/>
       <c r="E16" s="30" t="s">
         <v>10</v>
       </c>
@@ -4145,8 +4176,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="4"/>
-      <c r="C17" s="174"/>
-      <c r="D17" s="174"/>
+      <c r="C17" s="188"/>
+      <c r="D17" s="188"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -4165,10 +4196,10 @@
       <c r="C21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="175" t="s">
+      <c r="D21" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="175"/>
+      <c r="E21" s="189"/>
       <c r="F21" s="17" t="s">
         <v>16</v>
       </c>
@@ -4180,10 +4211,10 @@
       <c r="C22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="176" t="s">
+      <c r="D22" s="190" t="s">
         <v>123</v>
       </c>
-      <c r="E22" s="176"/>
+      <c r="E22" s="190"/>
       <c r="F22" s="20" t="s">
         <v>124</v>
       </c>
@@ -4240,8 +4271,8 @@
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="192"/>
-      <c r="E30" s="192"/>
+      <c r="D30" s="178"/>
+      <c r="E30" s="178"/>
       <c r="F30" s="26"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -4252,61 +4283,61 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="193" t="s">
+      <c r="B34" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="194"/>
-      <c r="D34" s="194"/>
-      <c r="E34" s="194"/>
-      <c r="F34" s="195"/>
+      <c r="C34" s="180"/>
+      <c r="D34" s="180"/>
+      <c r="E34" s="180"/>
+      <c r="F34" s="181"/>
     </row>
     <row r="35" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="171" t="s">
+      <c r="B35" s="185" t="s">
         <v>235</v>
       </c>
-      <c r="C35" s="172"/>
-      <c r="D35" s="172"/>
-      <c r="E35" s="172"/>
-      <c r="F35" s="173"/>
+      <c r="C35" s="186"/>
+      <c r="D35" s="186"/>
+      <c r="E35" s="186"/>
+      <c r="F35" s="187"/>
     </row>
     <row r="36" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="198" t="s">
+      <c r="B36" s="171" t="s">
         <v>236</v>
       </c>
-      <c r="C36" s="199"/>
-      <c r="D36" s="199"/>
-      <c r="E36" s="199"/>
-      <c r="F36" s="200"/>
+      <c r="C36" s="172"/>
+      <c r="D36" s="172"/>
+      <c r="E36" s="172"/>
+      <c r="F36" s="173"/>
       <c r="J36" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="198" t="s">
+      <c r="B37" s="171" t="s">
         <v>237</v>
       </c>
-      <c r="C37" s="199"/>
-      <c r="D37" s="199"/>
-      <c r="E37" s="199"/>
-      <c r="F37" s="200"/>
+      <c r="C37" s="172"/>
+      <c r="D37" s="172"/>
+      <c r="E37" s="172"/>
+      <c r="F37" s="173"/>
     </row>
     <row r="38" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="198" t="s">
+      <c r="B38" s="171" t="s">
         <v>238</v>
       </c>
-      <c r="C38" s="199"/>
-      <c r="D38" s="199"/>
-      <c r="E38" s="199"/>
-      <c r="F38" s="200"/>
+      <c r="C38" s="172"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="172"/>
+      <c r="F38" s="173"/>
     </row>
     <row r="39" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="189" t="s">
+      <c r="B39" s="174" t="s">
         <v>239</v>
       </c>
-      <c r="C39" s="190"/>
-      <c r="D39" s="190"/>
-      <c r="E39" s="190"/>
-      <c r="F39" s="191"/>
+      <c r="C39" s="175"/>
+      <c r="D39" s="175"/>
+      <c r="E39" s="175"/>
+      <c r="F39" s="176"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="7"/>
@@ -4467,18 +4498,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
@@ -4495,6 +4514,18 @@
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -4515,7 +4546,7 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="39.950000000000003" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="39.950000000000003" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="82" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="83" customWidth="1"/>
@@ -5618,14 +5649,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BR55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="6" ySplit="12" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="6.7109375" style="39" customWidth="1"/>
     <col min="2" max="2" width="50.7109375" style="31" customWidth="1"/>
@@ -5644,296 +5675,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="206"/>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
-      <c r="N1" s="206"/>
-      <c r="O1" s="206"/>
-      <c r="P1" s="206"/>
-      <c r="Q1" s="206"/>
-      <c r="R1" s="206"/>
-      <c r="S1" s="206"/>
-      <c r="T1" s="206"/>
-      <c r="U1" s="206"/>
-      <c r="V1" s="206"/>
-      <c r="W1" s="206"/>
-      <c r="X1" s="206"/>
-      <c r="Y1" s="206"/>
-      <c r="Z1" s="206"/>
-      <c r="AA1" s="206"/>
-      <c r="AB1" s="206"/>
-      <c r="AC1" s="206"/>
-      <c r="AD1" s="206"/>
-      <c r="AE1" s="206"/>
-      <c r="AF1" s="206"/>
-      <c r="AG1" s="206"/>
-      <c r="AH1" s="206"/>
-      <c r="AI1" s="206"/>
-      <c r="AJ1" s="206"/>
-      <c r="AK1" s="206"/>
-      <c r="AL1" s="206"/>
-      <c r="AM1" s="206"/>
-      <c r="AN1" s="206"/>
-      <c r="AO1" s="206"/>
-      <c r="AP1" s="206"/>
-      <c r="AQ1" s="206"/>
-      <c r="AR1" s="206"/>
-      <c r="AS1" s="206"/>
-      <c r="AT1" s="206"/>
-      <c r="AU1" s="206"/>
-      <c r="AV1" s="206"/>
-      <c r="AW1" s="206"/>
-      <c r="AX1" s="206"/>
-      <c r="AY1" s="206"/>
-      <c r="AZ1" s="206"/>
-      <c r="BA1" s="206"/>
-      <c r="BB1" s="206"/>
-      <c r="BC1" s="206"/>
-      <c r="BD1" s="206"/>
-      <c r="BE1" s="206"/>
-      <c r="BF1" s="206"/>
-      <c r="BG1" s="206"/>
-      <c r="BH1" s="206"/>
-      <c r="BI1" s="206"/>
-      <c r="BJ1" s="206"/>
-      <c r="BK1" s="206"/>
-      <c r="BL1" s="206"/>
-      <c r="BM1" s="206"/>
-      <c r="BN1" s="206"/>
-      <c r="BO1" s="206"/>
-      <c r="BP1" s="206"/>
-      <c r="BQ1" s="206"/>
-      <c r="BR1" s="206"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
+      <c r="N1" s="201"/>
+      <c r="O1" s="201"/>
+      <c r="P1" s="201"/>
+      <c r="Q1" s="201"/>
+      <c r="R1" s="201"/>
+      <c r="S1" s="201"/>
+      <c r="T1" s="201"/>
+      <c r="U1" s="201"/>
+      <c r="V1" s="201"/>
+      <c r="W1" s="201"/>
+      <c r="X1" s="201"/>
+      <c r="Y1" s="201"/>
+      <c r="Z1" s="201"/>
+      <c r="AA1" s="201"/>
+      <c r="AB1" s="201"/>
+      <c r="AC1" s="201"/>
+      <c r="AD1" s="201"/>
+      <c r="AE1" s="201"/>
+      <c r="AF1" s="201"/>
+      <c r="AG1" s="201"/>
+      <c r="AH1" s="201"/>
+      <c r="AI1" s="201"/>
+      <c r="AJ1" s="201"/>
+      <c r="AK1" s="201"/>
+      <c r="AL1" s="201"/>
+      <c r="AM1" s="201"/>
+      <c r="AN1" s="201"/>
+      <c r="AO1" s="201"/>
+      <c r="AP1" s="201"/>
+      <c r="AQ1" s="201"/>
+      <c r="AR1" s="201"/>
+      <c r="AS1" s="201"/>
+      <c r="AT1" s="201"/>
+      <c r="AU1" s="201"/>
+      <c r="AV1" s="201"/>
+      <c r="AW1" s="201"/>
+      <c r="AX1" s="201"/>
+      <c r="AY1" s="201"/>
+      <c r="AZ1" s="201"/>
+      <c r="BA1" s="201"/>
+      <c r="BB1" s="201"/>
+      <c r="BC1" s="201"/>
+      <c r="BD1" s="201"/>
+      <c r="BE1" s="201"/>
+      <c r="BF1" s="201"/>
+      <c r="BG1" s="201"/>
+      <c r="BH1" s="201"/>
+      <c r="BI1" s="201"/>
+      <c r="BJ1" s="201"/>
+      <c r="BK1" s="201"/>
+      <c r="BL1" s="201"/>
+      <c r="BM1" s="201"/>
+      <c r="BN1" s="201"/>
+      <c r="BO1" s="201"/>
+      <c r="BP1" s="201"/>
+      <c r="BQ1" s="201"/>
+      <c r="BR1" s="201"/>
     </row>
     <row r="2" spans="1:70" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="202" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="206"/>
-      <c r="I2" s="207"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="207"/>
-      <c r="P2" s="207"/>
-      <c r="Q2" s="207"/>
-      <c r="R2" s="207"/>
-      <c r="S2" s="207"/>
-      <c r="T2" s="207"/>
-      <c r="U2" s="207"/>
-      <c r="V2" s="207"/>
-      <c r="W2" s="207"/>
-      <c r="X2" s="207"/>
-      <c r="Y2" s="207"/>
-      <c r="Z2" s="207"/>
-      <c r="AA2" s="207"/>
-      <c r="AB2" s="207"/>
-      <c r="AC2" s="207"/>
-      <c r="AD2" s="207"/>
-      <c r="AE2" s="207"/>
-      <c r="AF2" s="207"/>
-      <c r="AG2" s="207"/>
-      <c r="AH2" s="207"/>
-      <c r="AI2" s="207"/>
-      <c r="AJ2" s="207"/>
-      <c r="AK2" s="207"/>
-      <c r="AL2" s="207"/>
-      <c r="AM2" s="207"/>
-      <c r="AN2" s="207"/>
-      <c r="AO2" s="207"/>
-      <c r="AP2" s="207"/>
-      <c r="AQ2" s="207"/>
-      <c r="AR2" s="207"/>
-      <c r="AS2" s="207"/>
-      <c r="AT2" s="207"/>
-      <c r="AU2" s="207"/>
-      <c r="AV2" s="207"/>
-      <c r="AW2" s="207"/>
-      <c r="AX2" s="207"/>
-      <c r="AY2" s="207"/>
-      <c r="AZ2" s="207"/>
-      <c r="BA2" s="207"/>
-      <c r="BB2" s="207"/>
-      <c r="BC2" s="207"/>
-      <c r="BD2" s="207"/>
-      <c r="BE2" s="207"/>
-      <c r="BF2" s="207"/>
-      <c r="BG2" s="207"/>
-      <c r="BH2" s="207"/>
-      <c r="BI2" s="207"/>
-      <c r="BJ2" s="207"/>
-      <c r="BK2" s="207"/>
-      <c r="BL2" s="207"/>
-      <c r="BM2" s="207"/>
-      <c r="BN2" s="207"/>
-      <c r="BO2" s="207"/>
-      <c r="BP2" s="207"/>
-      <c r="BQ2" s="207"/>
-      <c r="BR2" s="208"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="202"/>
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="202"/>
+      <c r="W2" s="202"/>
+      <c r="X2" s="202"/>
+      <c r="Y2" s="202"/>
+      <c r="Z2" s="202"/>
+      <c r="AA2" s="202"/>
+      <c r="AB2" s="202"/>
+      <c r="AC2" s="202"/>
+      <c r="AD2" s="202"/>
+      <c r="AE2" s="202"/>
+      <c r="AF2" s="202"/>
+      <c r="AG2" s="202"/>
+      <c r="AH2" s="202"/>
+      <c r="AI2" s="202"/>
+      <c r="AJ2" s="202"/>
+      <c r="AK2" s="202"/>
+      <c r="AL2" s="202"/>
+      <c r="AM2" s="202"/>
+      <c r="AN2" s="202"/>
+      <c r="AO2" s="202"/>
+      <c r="AP2" s="202"/>
+      <c r="AQ2" s="202"/>
+      <c r="AR2" s="202"/>
+      <c r="AS2" s="202"/>
+      <c r="AT2" s="202"/>
+      <c r="AU2" s="202"/>
+      <c r="AV2" s="202"/>
+      <c r="AW2" s="202"/>
+      <c r="AX2" s="202"/>
+      <c r="AY2" s="202"/>
+      <c r="AZ2" s="202"/>
+      <c r="BA2" s="202"/>
+      <c r="BB2" s="202"/>
+      <c r="BC2" s="202"/>
+      <c r="BD2" s="202"/>
+      <c r="BE2" s="202"/>
+      <c r="BF2" s="202"/>
+      <c r="BG2" s="202"/>
+      <c r="BH2" s="202"/>
+      <c r="BI2" s="202"/>
+      <c r="BJ2" s="202"/>
+      <c r="BK2" s="202"/>
+      <c r="BL2" s="202"/>
+      <c r="BM2" s="202"/>
+      <c r="BN2" s="202"/>
+      <c r="BO2" s="202"/>
+      <c r="BP2" s="202"/>
+      <c r="BQ2" s="202"/>
+      <c r="BR2" s="203"/>
     </row>
     <row r="3" spans="1:70" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="206"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="207"/>
-      <c r="Q3" s="207"/>
-      <c r="R3" s="207"/>
-      <c r="S3" s="207"/>
-      <c r="T3" s="207"/>
-      <c r="U3" s="207"/>
-      <c r="V3" s="207"/>
-      <c r="W3" s="207"/>
-      <c r="X3" s="207"/>
-      <c r="Y3" s="207"/>
-      <c r="Z3" s="207"/>
-      <c r="AA3" s="207"/>
-      <c r="AB3" s="207"/>
-      <c r="AC3" s="207"/>
-      <c r="AD3" s="207"/>
-      <c r="AE3" s="207"/>
-      <c r="AF3" s="207"/>
-      <c r="AG3" s="207"/>
-      <c r="AH3" s="207"/>
-      <c r="AI3" s="207"/>
-      <c r="AJ3" s="207"/>
-      <c r="AK3" s="207"/>
-      <c r="AL3" s="207"/>
-      <c r="AM3" s="207"/>
-      <c r="AN3" s="207"/>
-      <c r="AO3" s="207"/>
-      <c r="AP3" s="207"/>
-      <c r="AQ3" s="207"/>
-      <c r="AR3" s="207"/>
-      <c r="AS3" s="207"/>
-      <c r="AT3" s="207"/>
-      <c r="AU3" s="207"/>
-      <c r="AV3" s="207"/>
-      <c r="AW3" s="207"/>
-      <c r="AX3" s="207"/>
-      <c r="AY3" s="207"/>
-      <c r="AZ3" s="207"/>
-      <c r="BA3" s="207"/>
-      <c r="BB3" s="207"/>
-      <c r="BC3" s="207"/>
-      <c r="BD3" s="207"/>
-      <c r="BE3" s="207"/>
-      <c r="BF3" s="207"/>
-      <c r="BG3" s="207"/>
-      <c r="BH3" s="207"/>
-      <c r="BI3" s="207"/>
-      <c r="BJ3" s="207"/>
-      <c r="BK3" s="207"/>
-      <c r="BL3" s="207"/>
-      <c r="BM3" s="207"/>
-      <c r="BN3" s="207"/>
-      <c r="BO3" s="207"/>
-      <c r="BP3" s="207"/>
-      <c r="BQ3" s="207"/>
-      <c r="BR3" s="208"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202"/>
+      <c r="Q3" s="202"/>
+      <c r="R3" s="202"/>
+      <c r="S3" s="202"/>
+      <c r="T3" s="202"/>
+      <c r="U3" s="202"/>
+      <c r="V3" s="202"/>
+      <c r="W3" s="202"/>
+      <c r="X3" s="202"/>
+      <c r="Y3" s="202"/>
+      <c r="Z3" s="202"/>
+      <c r="AA3" s="202"/>
+      <c r="AB3" s="202"/>
+      <c r="AC3" s="202"/>
+      <c r="AD3" s="202"/>
+      <c r="AE3" s="202"/>
+      <c r="AF3" s="202"/>
+      <c r="AG3" s="202"/>
+      <c r="AH3" s="202"/>
+      <c r="AI3" s="202"/>
+      <c r="AJ3" s="202"/>
+      <c r="AK3" s="202"/>
+      <c r="AL3" s="202"/>
+      <c r="AM3" s="202"/>
+      <c r="AN3" s="202"/>
+      <c r="AO3" s="202"/>
+      <c r="AP3" s="202"/>
+      <c r="AQ3" s="202"/>
+      <c r="AR3" s="202"/>
+      <c r="AS3" s="202"/>
+      <c r="AT3" s="202"/>
+      <c r="AU3" s="202"/>
+      <c r="AV3" s="202"/>
+      <c r="AW3" s="202"/>
+      <c r="AX3" s="202"/>
+      <c r="AY3" s="202"/>
+      <c r="AZ3" s="202"/>
+      <c r="BA3" s="202"/>
+      <c r="BB3" s="202"/>
+      <c r="BC3" s="202"/>
+      <c r="BD3" s="202"/>
+      <c r="BE3" s="202"/>
+      <c r="BF3" s="202"/>
+      <c r="BG3" s="202"/>
+      <c r="BH3" s="202"/>
+      <c r="BI3" s="202"/>
+      <c r="BJ3" s="202"/>
+      <c r="BK3" s="202"/>
+      <c r="BL3" s="202"/>
+      <c r="BM3" s="202"/>
+      <c r="BN3" s="202"/>
+      <c r="BO3" s="202"/>
+      <c r="BP3" s="202"/>
+      <c r="BQ3" s="202"/>
+      <c r="BR3" s="203"/>
     </row>
     <row r="4" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A4" s="209"/>
-      <c r="B4" s="209"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="209"/>
-      <c r="I4" s="209"/>
-      <c r="J4" s="209"/>
-      <c r="K4" s="209"/>
-      <c r="L4" s="209"/>
-      <c r="M4" s="209"/>
-      <c r="N4" s="209"/>
-      <c r="O4" s="209"/>
-      <c r="P4" s="209"/>
-      <c r="Q4" s="209"/>
-      <c r="R4" s="209"/>
-      <c r="S4" s="209"/>
-      <c r="T4" s="209"/>
-      <c r="U4" s="209"/>
-      <c r="V4" s="209"/>
-      <c r="W4" s="209"/>
-      <c r="X4" s="209"/>
-      <c r="Y4" s="209"/>
-      <c r="Z4" s="209"/>
-      <c r="AA4" s="209"/>
-      <c r="AB4" s="209"/>
-      <c r="AC4" s="209"/>
-      <c r="AD4" s="209"/>
-      <c r="AE4" s="209"/>
-      <c r="AF4" s="209"/>
-      <c r="AG4" s="209"/>
-      <c r="AH4" s="209"/>
-      <c r="AI4" s="209"/>
-      <c r="AJ4" s="209"/>
-      <c r="AK4" s="209"/>
-      <c r="AL4" s="209"/>
-      <c r="AM4" s="209"/>
-      <c r="AN4" s="209"/>
-      <c r="AO4" s="209"/>
-      <c r="AP4" s="209"/>
-      <c r="AQ4" s="209"/>
-      <c r="AR4" s="209"/>
-      <c r="AS4" s="209"/>
-      <c r="AT4" s="209"/>
-      <c r="AU4" s="209"/>
-      <c r="AV4" s="209"/>
-      <c r="AW4" s="209"/>
-      <c r="AX4" s="209"/>
-      <c r="AY4" s="209"/>
-      <c r="AZ4" s="209"/>
-      <c r="BA4" s="209"/>
-      <c r="BB4" s="209"/>
-      <c r="BC4" s="209"/>
-      <c r="BD4" s="209"/>
-      <c r="BE4" s="209"/>
-      <c r="BF4" s="209"/>
-      <c r="BG4" s="209"/>
-      <c r="BH4" s="209"/>
-      <c r="BI4" s="209"/>
-      <c r="BJ4" s="209"/>
-      <c r="BK4" s="209"/>
-      <c r="BL4" s="209"/>
-      <c r="BM4" s="209"/>
-      <c r="BN4" s="209"/>
-      <c r="BO4" s="209"/>
-      <c r="BP4" s="209"/>
-      <c r="BQ4" s="209"/>
-      <c r="BR4" s="210"/>
+      <c r="A4" s="204"/>
+      <c r="B4" s="204"/>
+      <c r="C4" s="204"/>
+      <c r="D4" s="204"/>
+      <c r="E4" s="204"/>
+      <c r="F4" s="204"/>
+      <c r="G4" s="204"/>
+      <c r="H4" s="204"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
+      <c r="K4" s="204"/>
+      <c r="L4" s="204"/>
+      <c r="M4" s="204"/>
+      <c r="N4" s="204"/>
+      <c r="O4" s="204"/>
+      <c r="P4" s="204"/>
+      <c r="Q4" s="204"/>
+      <c r="R4" s="204"/>
+      <c r="S4" s="204"/>
+      <c r="T4" s="204"/>
+      <c r="U4" s="204"/>
+      <c r="V4" s="204"/>
+      <c r="W4" s="204"/>
+      <c r="X4" s="204"/>
+      <c r="Y4" s="204"/>
+      <c r="Z4" s="204"/>
+      <c r="AA4" s="204"/>
+      <c r="AB4" s="204"/>
+      <c r="AC4" s="204"/>
+      <c r="AD4" s="204"/>
+      <c r="AE4" s="204"/>
+      <c r="AF4" s="204"/>
+      <c r="AG4" s="204"/>
+      <c r="AH4" s="204"/>
+      <c r="AI4" s="204"/>
+      <c r="AJ4" s="204"/>
+      <c r="AK4" s="204"/>
+      <c r="AL4" s="204"/>
+      <c r="AM4" s="204"/>
+      <c r="AN4" s="204"/>
+      <c r="AO4" s="204"/>
+      <c r="AP4" s="204"/>
+      <c r="AQ4" s="204"/>
+      <c r="AR4" s="204"/>
+      <c r="AS4" s="204"/>
+      <c r="AT4" s="204"/>
+      <c r="AU4" s="204"/>
+      <c r="AV4" s="204"/>
+      <c r="AW4" s="204"/>
+      <c r="AX4" s="204"/>
+      <c r="AY4" s="204"/>
+      <c r="AZ4" s="204"/>
+      <c r="BA4" s="204"/>
+      <c r="BB4" s="204"/>
+      <c r="BC4" s="204"/>
+      <c r="BD4" s="204"/>
+      <c r="BE4" s="204"/>
+      <c r="BF4" s="204"/>
+      <c r="BG4" s="204"/>
+      <c r="BH4" s="204"/>
+      <c r="BI4" s="204"/>
+      <c r="BJ4" s="204"/>
+      <c r="BK4" s="204"/>
+      <c r="BL4" s="204"/>
+      <c r="BM4" s="204"/>
+      <c r="BN4" s="204"/>
+      <c r="BO4" s="204"/>
+      <c r="BP4" s="204"/>
+      <c r="BQ4" s="204"/>
+      <c r="BR4" s="205"/>
     </row>
     <row r="5" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickTop="1">
       <c r="A5" s="113"/>
@@ -6048,11 +6079,11 @@
         <v>25</v>
       </c>
       <c r="C8" s="126"/>
-      <c r="D8" s="205">
+      <c r="D8" s="215">
         <v>45486</v>
       </c>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="K8" s="138" t="s">
@@ -6061,179 +6092,179 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="O8" s="202" t="str">
+      <c r="O8" s="210" t="str">
         <f>"Semana "&amp;(O10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 1</v>
       </c>
-      <c r="P8" s="203"/>
-      <c r="Q8" s="203"/>
-      <c r="R8" s="203"/>
-      <c r="S8" s="203"/>
-      <c r="T8" s="203"/>
-      <c r="U8" s="204"/>
-      <c r="V8" s="202" t="str">
+      <c r="P8" s="211"/>
+      <c r="Q8" s="211"/>
+      <c r="R8" s="211"/>
+      <c r="S8" s="211"/>
+      <c r="T8" s="211"/>
+      <c r="U8" s="212"/>
+      <c r="V8" s="210" t="str">
         <f>"Semana "&amp;(V10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 2</v>
       </c>
-      <c r="W8" s="203"/>
-      <c r="X8" s="203"/>
-      <c r="Y8" s="203"/>
-      <c r="Z8" s="203"/>
-      <c r="AA8" s="203"/>
-      <c r="AB8" s="204"/>
-      <c r="AC8" s="202" t="str">
+      <c r="W8" s="211"/>
+      <c r="X8" s="211"/>
+      <c r="Y8" s="211"/>
+      <c r="Z8" s="211"/>
+      <c r="AA8" s="211"/>
+      <c r="AB8" s="212"/>
+      <c r="AC8" s="210" t="str">
         <f>"Semana "&amp;(AC10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 3</v>
       </c>
-      <c r="AD8" s="203"/>
-      <c r="AE8" s="203"/>
-      <c r="AF8" s="203"/>
-      <c r="AG8" s="203"/>
-      <c r="AH8" s="203"/>
-      <c r="AI8" s="204"/>
-      <c r="AJ8" s="202" t="str">
+      <c r="AD8" s="211"/>
+      <c r="AE8" s="211"/>
+      <c r="AF8" s="211"/>
+      <c r="AG8" s="211"/>
+      <c r="AH8" s="211"/>
+      <c r="AI8" s="212"/>
+      <c r="AJ8" s="210" t="str">
         <f>"Semana "&amp;(AJ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 4</v>
       </c>
-      <c r="AK8" s="203"/>
-      <c r="AL8" s="203"/>
-      <c r="AM8" s="203"/>
-      <c r="AN8" s="203"/>
-      <c r="AO8" s="203"/>
-      <c r="AP8" s="204"/>
-      <c r="AQ8" s="202" t="str">
+      <c r="AK8" s="211"/>
+      <c r="AL8" s="211"/>
+      <c r="AM8" s="211"/>
+      <c r="AN8" s="211"/>
+      <c r="AO8" s="211"/>
+      <c r="AP8" s="212"/>
+      <c r="AQ8" s="210" t="str">
         <f>"Semana "&amp;(AQ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 5</v>
       </c>
-      <c r="AR8" s="203"/>
-      <c r="AS8" s="203"/>
-      <c r="AT8" s="203"/>
-      <c r="AU8" s="203"/>
-      <c r="AV8" s="203"/>
-      <c r="AW8" s="204"/>
-      <c r="AX8" s="202" t="str">
+      <c r="AR8" s="211"/>
+      <c r="AS8" s="211"/>
+      <c r="AT8" s="211"/>
+      <c r="AU8" s="211"/>
+      <c r="AV8" s="211"/>
+      <c r="AW8" s="212"/>
+      <c r="AX8" s="210" t="str">
         <f>"Semana "&amp;(AX10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 6</v>
       </c>
-      <c r="AY8" s="203"/>
-      <c r="AZ8" s="203"/>
-      <c r="BA8" s="203"/>
-      <c r="BB8" s="203"/>
-      <c r="BC8" s="203"/>
-      <c r="BD8" s="204"/>
-      <c r="BE8" s="202" t="str">
+      <c r="AY8" s="211"/>
+      <c r="AZ8" s="211"/>
+      <c r="BA8" s="211"/>
+      <c r="BB8" s="211"/>
+      <c r="BC8" s="211"/>
+      <c r="BD8" s="212"/>
+      <c r="BE8" s="210" t="str">
         <f>"Semana "&amp;(BE10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 7</v>
       </c>
-      <c r="BF8" s="203"/>
-      <c r="BG8" s="203"/>
-      <c r="BH8" s="203"/>
-      <c r="BI8" s="203"/>
-      <c r="BJ8" s="203"/>
-      <c r="BK8" s="204"/>
-      <c r="BL8" s="202" t="str">
+      <c r="BF8" s="211"/>
+      <c r="BG8" s="211"/>
+      <c r="BH8" s="211"/>
+      <c r="BI8" s="211"/>
+      <c r="BJ8" s="211"/>
+      <c r="BK8" s="212"/>
+      <c r="BL8" s="210" t="str">
         <f>"Semana "&amp;(BL10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 8</v>
       </c>
-      <c r="BM8" s="203"/>
-      <c r="BN8" s="203"/>
-      <c r="BO8" s="203"/>
-      <c r="BP8" s="203"/>
-      <c r="BQ8" s="203"/>
-      <c r="BR8" s="215"/>
+      <c r="BM8" s="211"/>
+      <c r="BN8" s="211"/>
+      <c r="BO8" s="211"/>
+      <c r="BP8" s="211"/>
+      <c r="BQ8" s="211"/>
+      <c r="BR8" s="213"/>
     </row>
     <row r="9" spans="1:70" ht="17.25" customHeight="1">
       <c r="B9" s="125" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="126"/>
-      <c r="D9" s="201" t="s">
+      <c r="D9" s="214" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="201"/>
-      <c r="F9" s="201"/>
+      <c r="E9" s="214"/>
+      <c r="F9" s="214"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="O9" s="211">
+      <c r="O9" s="206">
         <f>O10</f>
         <v>45481</v>
       </c>
-      <c r="P9" s="212"/>
-      <c r="Q9" s="212"/>
-      <c r="R9" s="212"/>
-      <c r="S9" s="212"/>
-      <c r="T9" s="212"/>
-      <c r="U9" s="213"/>
-      <c r="V9" s="211">
+      <c r="P9" s="207"/>
+      <c r="Q9" s="207"/>
+      <c r="R9" s="207"/>
+      <c r="S9" s="207"/>
+      <c r="T9" s="207"/>
+      <c r="U9" s="208"/>
+      <c r="V9" s="206">
         <f>V10</f>
         <v>45488</v>
       </c>
-      <c r="W9" s="212"/>
-      <c r="X9" s="212"/>
-      <c r="Y9" s="212"/>
-      <c r="Z9" s="212"/>
-      <c r="AA9" s="212"/>
-      <c r="AB9" s="213"/>
-      <c r="AC9" s="211">
+      <c r="W9" s="207"/>
+      <c r="X9" s="207"/>
+      <c r="Y9" s="207"/>
+      <c r="Z9" s="207"/>
+      <c r="AA9" s="207"/>
+      <c r="AB9" s="208"/>
+      <c r="AC9" s="206">
         <f>AC10</f>
         <v>45495</v>
       </c>
-      <c r="AD9" s="212"/>
-      <c r="AE9" s="212"/>
-      <c r="AF9" s="212"/>
-      <c r="AG9" s="212"/>
-      <c r="AH9" s="212"/>
-      <c r="AI9" s="213"/>
-      <c r="AJ9" s="211">
+      <c r="AD9" s="207"/>
+      <c r="AE9" s="207"/>
+      <c r="AF9" s="207"/>
+      <c r="AG9" s="207"/>
+      <c r="AH9" s="207"/>
+      <c r="AI9" s="208"/>
+      <c r="AJ9" s="206">
         <f>AJ10</f>
         <v>45502</v>
       </c>
-      <c r="AK9" s="212"/>
-      <c r="AL9" s="212"/>
-      <c r="AM9" s="212"/>
-      <c r="AN9" s="212"/>
-      <c r="AO9" s="212"/>
-      <c r="AP9" s="213"/>
-      <c r="AQ9" s="211">
+      <c r="AK9" s="207"/>
+      <c r="AL9" s="207"/>
+      <c r="AM9" s="207"/>
+      <c r="AN9" s="207"/>
+      <c r="AO9" s="207"/>
+      <c r="AP9" s="208"/>
+      <c r="AQ9" s="206">
         <f>AQ10</f>
         <v>45509</v>
       </c>
-      <c r="AR9" s="212"/>
-      <c r="AS9" s="212"/>
-      <c r="AT9" s="212"/>
-      <c r="AU9" s="212"/>
-      <c r="AV9" s="212"/>
-      <c r="AW9" s="213"/>
-      <c r="AX9" s="211">
+      <c r="AR9" s="207"/>
+      <c r="AS9" s="207"/>
+      <c r="AT9" s="207"/>
+      <c r="AU9" s="207"/>
+      <c r="AV9" s="207"/>
+      <c r="AW9" s="208"/>
+      <c r="AX9" s="206">
         <f>AX10</f>
         <v>45516</v>
       </c>
-      <c r="AY9" s="212"/>
-      <c r="AZ9" s="212"/>
-      <c r="BA9" s="212"/>
-      <c r="BB9" s="212"/>
-      <c r="BC9" s="212"/>
-      <c r="BD9" s="213"/>
-      <c r="BE9" s="211">
+      <c r="AY9" s="207"/>
+      <c r="AZ9" s="207"/>
+      <c r="BA9" s="207"/>
+      <c r="BB9" s="207"/>
+      <c r="BC9" s="207"/>
+      <c r="BD9" s="208"/>
+      <c r="BE9" s="206">
         <f>BE10</f>
         <v>45523</v>
       </c>
-      <c r="BF9" s="212"/>
-      <c r="BG9" s="212"/>
-      <c r="BH9" s="212"/>
-      <c r="BI9" s="212"/>
-      <c r="BJ9" s="212"/>
-      <c r="BK9" s="213"/>
-      <c r="BL9" s="211">
+      <c r="BF9" s="207"/>
+      <c r="BG9" s="207"/>
+      <c r="BH9" s="207"/>
+      <c r="BI9" s="207"/>
+      <c r="BJ9" s="207"/>
+      <c r="BK9" s="208"/>
+      <c r="BL9" s="206">
         <f>BL10</f>
         <v>45530</v>
       </c>
-      <c r="BM9" s="212"/>
-      <c r="BN9" s="212"/>
-      <c r="BO9" s="212"/>
-      <c r="BP9" s="212"/>
-      <c r="BQ9" s="212"/>
-      <c r="BR9" s="214"/>
+      <c r="BM9" s="207"/>
+      <c r="BN9" s="207"/>
+      <c r="BO9" s="207"/>
+      <c r="BP9" s="207"/>
+      <c r="BQ9" s="207"/>
+      <c r="BR9" s="209"/>
     </row>
     <row r="10" spans="1:70">
       <c r="O10" s="33">
@@ -6836,12 +6867,13 @@
       <c r="F13" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="G13" s="90"/>
+      <c r="G13" s="90" t="s">
+        <v>241</v>
+      </c>
       <c r="H13" s="49"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="50" t="str">
-        <f t="shared" ref="J13:J19" si="46">IF(ISBLANK(I13)," - ",IF(K13=0,I13,I13+K13-1))</f>
-        <v xml:space="preserve"> - </v>
+      <c r="J13" s="50" t="s">
+        <v>242</v>
       </c>
       <c r="K13" s="53">
         <v>0</v>
@@ -6850,7 +6882,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="54" t="str">
-        <f t="shared" ref="M13:M19" si="47">IF(OR(J13=0,I13=0)," - ",NETWORKDAYS(I13,J13))</f>
+        <f t="shared" ref="M13:M19" si="46">IF(OR(J13=0,I13=0)," - ",NETWORKDAYS(I13,J13))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N13" s="137"/>
@@ -6931,11 +6963,13 @@
       <c r="F14" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="G14" s="90"/>
+      <c r="G14" s="90" t="s">
+        <v>244</v>
+      </c>
       <c r="H14" s="49"/>
       <c r="I14" s="51"/>
       <c r="J14" s="50" t="str">
-        <f t="shared" ref="J14" si="48">IF(ISBLANK(I14)," - ",IF(K14=0,I14,I14+K14-1))</f>
+        <f t="shared" ref="J14" si="47">IF(ISBLANK(I14)," - ",IF(K14=0,I14,I14+K14-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K14" s="53">
@@ -6945,7 +6979,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="54" t="str">
-        <f t="shared" ref="M14" si="49">IF(OR(J14=0,I14=0)," - ",NETWORKDAYS(I14,J14))</f>
+        <f t="shared" ref="M14" si="48">IF(OR(J14=0,I14=0)," - ",NETWORKDAYS(I14,J14))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N14" s="137"/>
@@ -7026,11 +7060,13 @@
       <c r="F15" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="G15" s="90"/>
+      <c r="G15" s="90" t="s">
+        <v>244</v>
+      </c>
       <c r="H15" s="49"/>
       <c r="I15" s="51"/>
       <c r="J15" s="50" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="J13:J19" si="49">IF(ISBLANK(I15)," - ",IF(K15=0,I15,I15+K15-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K15" s="53">
@@ -7040,7 +7076,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="54" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N15" s="137"/>
@@ -7121,12 +7157,13 @@
       <c r="F16" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="90"/>
+      <c r="G16" s="90" t="s">
+        <v>243</v>
+      </c>
       <c r="H16" s="49"/>
       <c r="I16" s="51"/>
-      <c r="J16" s="50" t="str">
-        <f t="shared" ref="J16" si="50">IF(ISBLANK(I16)," - ",IF(K16=0,I16,I16+K16-1))</f>
-        <v xml:space="preserve"> - </v>
+      <c r="J16" s="50">
+        <v>20</v>
       </c>
       <c r="K16" s="53">
         <v>0</v>
@@ -7135,7 +7172,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="54" t="str">
-        <f t="shared" ref="M16" si="51">IF(OR(J16=0,I16=0)," - ",NETWORKDAYS(I16,J16))</f>
+        <f t="shared" ref="M16" si="50">IF(OR(J16=0,I16=0)," - ",NETWORKDAYS(I16,J16))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N16" s="135"/>
@@ -7216,12 +7253,13 @@
       <c r="F17" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="G17" s="90"/>
+      <c r="G17" s="90" t="s">
+        <v>243</v>
+      </c>
       <c r="H17" s="49"/>
       <c r="I17" s="51"/>
-      <c r="J17" s="50" t="str">
-        <f t="shared" si="46"/>
-        <v xml:space="preserve"> - </v>
+      <c r="J17" s="50">
+        <v>20</v>
       </c>
       <c r="K17" s="53">
         <v>0</v>
@@ -7230,7 +7268,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="54" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N17" s="135"/>
@@ -7311,12 +7349,13 @@
       <c r="F18" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="G18" s="91"/>
+      <c r="G18" s="91" t="s">
+        <v>246</v>
+      </c>
       <c r="H18" s="85"/>
       <c r="I18" s="89"/>
-      <c r="J18" s="50" t="str">
-        <f t="shared" si="46"/>
-        <v xml:space="preserve"> - </v>
+      <c r="J18" s="50">
+        <v>20</v>
       </c>
       <c r="K18" s="53">
         <v>0</v>
@@ -7325,7 +7364,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="54" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N18" s="136"/>
@@ -7406,12 +7445,13 @@
       <c r="F19" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="90"/>
+      <c r="G19" s="90" t="s">
+        <v>245</v>
+      </c>
       <c r="H19" s="49"/>
       <c r="I19" s="51"/>
-      <c r="J19" s="50" t="str">
-        <f t="shared" si="46"/>
-        <v xml:space="preserve"> - </v>
+      <c r="J19" s="50">
+        <v>20</v>
       </c>
       <c r="K19" s="53">
         <v>0</v>
@@ -7420,7 +7460,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="54" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N19" s="137"/>
@@ -7501,12 +7541,13 @@
       <c r="F20" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="G20" s="90"/>
+      <c r="G20" s="90" t="s">
+        <v>245</v>
+      </c>
       <c r="H20" s="49"/>
       <c r="I20" s="51"/>
-      <c r="J20" s="50" t="str">
-        <f t="shared" ref="J20:J21" si="52">IF(ISBLANK(I20)," - ",IF(K20=0,I20,I20+K20-1))</f>
-        <v xml:space="preserve"> - </v>
+      <c r="J20" s="50">
+        <v>20</v>
       </c>
       <c r="K20" s="53">
         <v>0</v>
@@ -7515,7 +7556,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="54" t="str">
-        <f t="shared" ref="M20:M21" si="53">IF(OR(J20=0,I20=0)," - ",NETWORKDAYS(I20,J20))</f>
+        <f t="shared" ref="M20:M21" si="51">IF(OR(J20=0,I20=0)," - ",NETWORKDAYS(I20,J20))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N20" s="137"/>
@@ -7596,12 +7637,13 @@
       <c r="F21" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="G21" s="90"/>
+      <c r="G21" s="90" t="s">
+        <v>246</v>
+      </c>
       <c r="H21" s="49"/>
       <c r="I21" s="51"/>
-      <c r="J21" s="50" t="str">
-        <f t="shared" si="52"/>
-        <v xml:space="preserve"> - </v>
+      <c r="J21" s="50">
+        <v>20</v>
       </c>
       <c r="K21" s="53">
         <v>0</v>
@@ -7610,7 +7652,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="54" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="51"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N21" s="135"/>
@@ -7689,7 +7731,7 @@
       <c r="H22" s="69"/>
       <c r="I22" s="70"/>
       <c r="J22" s="70" t="str">
-        <f t="shared" ref="J22:J54" si="54">IF(ISBLANK(I22)," - ",IF(K22=0,I22,I22+K22-1))</f>
+        <f t="shared" ref="J22:J54" si="52">IF(ISBLANK(I22)," - ",IF(K22=0,I22,I22+K22-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K22" s="71"/>
@@ -7780,7 +7822,7 @@
       <c r="H23" s="49"/>
       <c r="I23" s="51"/>
       <c r="J23" s="50" t="str">
-        <f t="shared" ref="J23:J26" si="55">IF(ISBLANK(I23)," - ",IF(K23=0,I23,I23+K23-1))</f>
+        <f t="shared" ref="J23:J26" si="53">IF(ISBLANK(I23)," - ",IF(K23=0,I23,I23+K23-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K23" s="53">
@@ -7875,7 +7917,7 @@
       <c r="H24" s="49"/>
       <c r="I24" s="51"/>
       <c r="J24" s="50" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K24" s="53">
@@ -7970,7 +8012,7 @@
       <c r="H25" s="49"/>
       <c r="I25" s="51"/>
       <c r="J25" s="50" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K25" s="53">
@@ -8065,7 +8107,7 @@
       <c r="H26" s="49"/>
       <c r="I26" s="51"/>
       <c r="J26" s="50" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="53"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K26" s="53">
@@ -8160,7 +8202,7 @@
       <c r="H27" s="49"/>
       <c r="I27" s="51"/>
       <c r="J27" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K27" s="53">
@@ -8170,7 +8212,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="54" t="str">
-        <f t="shared" ref="M27:M34" si="56">IF(OR(J27=0,I27=0)," - ",NETWORKDAYS(I27,J27))</f>
+        <f t="shared" ref="M27:M34" si="54">IF(OR(J27=0,I27=0)," - ",NETWORKDAYS(I27,J27))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N27" s="135"/>
@@ -8255,7 +8297,7 @@
       <c r="H28" s="49"/>
       <c r="I28" s="51"/>
       <c r="J28" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K28" s="53">
@@ -8265,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N28" s="135"/>
@@ -8350,7 +8392,7 @@
       <c r="H29" s="49"/>
       <c r="I29" s="51"/>
       <c r="J29" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K29" s="53">
@@ -8360,7 +8402,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N29" s="135"/>
@@ -8445,7 +8487,7 @@
       <c r="H30" s="49"/>
       <c r="I30" s="51"/>
       <c r="J30" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K30" s="53">
@@ -8455,7 +8497,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N30" s="135"/>
@@ -8540,7 +8582,7 @@
       <c r="H31" s="49"/>
       <c r="I31" s="51"/>
       <c r="J31" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K31" s="53">
@@ -8550,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N31" s="135"/>
@@ -8635,7 +8677,7 @@
       <c r="H32" s="49"/>
       <c r="I32" s="51"/>
       <c r="J32" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K32" s="53">
@@ -8645,7 +8687,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N32" s="135"/>
@@ -8730,7 +8772,7 @@
       <c r="H33" s="49"/>
       <c r="I33" s="51"/>
       <c r="J33" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K33" s="53">
@@ -8740,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N33" s="135"/>
@@ -8825,7 +8867,7 @@
       <c r="H34" s="49"/>
       <c r="I34" s="51"/>
       <c r="J34" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K34" s="53">
@@ -8835,7 +8877,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="54" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="54"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N34" s="135"/>
@@ -8920,7 +8962,7 @@
       <c r="H35" s="49"/>
       <c r="I35" s="51"/>
       <c r="J35" s="50" t="str">
-        <f t="shared" ref="J35" si="57">IF(ISBLANK(I35)," - ",IF(K35=0,I35,I35+K35-1))</f>
+        <f t="shared" ref="J35" si="55">IF(ISBLANK(I35)," - ",IF(K35=0,I35,I35+K35-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K35" s="53">
@@ -8930,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="54" t="str">
-        <f t="shared" ref="M35" si="58">IF(OR(J35=0,I35=0)," - ",NETWORKDAYS(I35,J35))</f>
+        <f t="shared" ref="M35" si="56">IF(OR(J35=0,I35=0)," - ",NETWORKDAYS(I35,J35))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="N35" s="135"/>
@@ -9009,7 +9051,7 @@
       <c r="H36" s="59"/>
       <c r="I36" s="60"/>
       <c r="J36" s="60" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K36" s="61"/>
@@ -9100,7 +9142,7 @@
       <c r="H37" s="49"/>
       <c r="I37" s="51"/>
       <c r="J37" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K37" s="53">
@@ -9195,7 +9237,7 @@
       <c r="H38" s="49"/>
       <c r="I38" s="51"/>
       <c r="J38" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K38" s="53">
@@ -9290,7 +9332,7 @@
       <c r="H39" s="49"/>
       <c r="I39" s="51"/>
       <c r="J39" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K39" s="53">
@@ -9385,7 +9427,7 @@
       <c r="H40" s="49"/>
       <c r="I40" s="51"/>
       <c r="J40" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K40" s="53">
@@ -9480,7 +9522,7 @@
       <c r="H41" s="49"/>
       <c r="I41" s="51"/>
       <c r="J41" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K41" s="53">
@@ -9575,7 +9617,7 @@
       <c r="H42" s="49"/>
       <c r="I42" s="51"/>
       <c r="J42" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K42" s="53">
@@ -9670,7 +9712,7 @@
       <c r="H43" s="49"/>
       <c r="I43" s="51"/>
       <c r="J43" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K43" s="53">
@@ -9765,7 +9807,7 @@
       <c r="H44" s="49"/>
       <c r="I44" s="51"/>
       <c r="J44" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K44" s="53">
@@ -9860,7 +9902,7 @@
       <c r="H45" s="49"/>
       <c r="I45" s="51"/>
       <c r="J45" s="50" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K45" s="53">
@@ -9955,7 +9997,7 @@
       <c r="H46" s="49"/>
       <c r="I46" s="51"/>
       <c r="J46" s="50" t="str">
-        <f t="shared" ref="J46" si="59">IF(ISBLANK(I46)," - ",IF(K46=0,I46,I46+K46-1))</f>
+        <f t="shared" ref="J46" si="57">IF(ISBLANK(I46)," - ",IF(K46=0,I46,I46+K46-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K46" s="53">
@@ -10044,7 +10086,7 @@
       <c r="H47" s="59"/>
       <c r="I47" s="60"/>
       <c r="J47" s="60" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K47" s="61"/>
@@ -10113,7 +10155,7 @@
     </row>
     <row r="48" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A48" s="92" t="str">
-        <f t="shared" ref="A48:A54" si="60">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A48:A54" si="58">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B48" s="46" t="s">
@@ -10135,7 +10177,7 @@
       <c r="H48" s="49"/>
       <c r="I48" s="51"/>
       <c r="J48" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K48" s="53">
@@ -10208,7 +10250,7 @@
     </row>
     <row r="49" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A49" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.2</v>
       </c>
       <c r="B49" s="46" t="s">
@@ -10230,7 +10272,7 @@
       <c r="H49" s="49"/>
       <c r="I49" s="51"/>
       <c r="J49" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K49" s="53">
@@ -10303,7 +10345,7 @@
     </row>
     <row r="50" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A50" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.3</v>
       </c>
       <c r="B50" s="46" t="s">
@@ -10325,7 +10367,7 @@
       <c r="H50" s="49"/>
       <c r="I50" s="51"/>
       <c r="J50" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K50" s="53">
@@ -10398,7 +10440,7 @@
     </row>
     <row r="51" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A51" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.4</v>
       </c>
       <c r="B51" s="46" t="s">
@@ -10420,7 +10462,7 @@
       <c r="H51" s="49"/>
       <c r="I51" s="51"/>
       <c r="J51" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K51" s="53">
@@ -10493,7 +10535,7 @@
     </row>
     <row r="52" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A52" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.5</v>
       </c>
       <c r="B52" s="46" t="s">
@@ -10515,7 +10557,7 @@
       <c r="H52" s="49"/>
       <c r="I52" s="51"/>
       <c r="J52" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K52" s="53">
@@ -10588,7 +10630,7 @@
     </row>
     <row r="53" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1">
       <c r="A53" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.6</v>
       </c>
       <c r="B53" s="46" t="s">
@@ -10610,7 +10652,7 @@
       <c r="H53" s="49"/>
       <c r="I53" s="51"/>
       <c r="J53" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K53" s="53">
@@ -10683,7 +10725,7 @@
     </row>
     <row r="54" spans="1:70" s="76" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A54" s="92" t="str">
-        <f t="shared" si="60"/>
+        <f t="shared" si="58"/>
         <v>4.7</v>
       </c>
       <c r="B54" s="46" t="s">
@@ -10705,7 +10747,7 @@
       <c r="H54" s="49"/>
       <c r="I54" s="51"/>
       <c r="J54" s="104" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="52"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="K54" s="53">
@@ -10852,6 +10894,12 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A11:M54" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="22">
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="O8:U8"/>
+    <mergeCell ref="V8:AB8"/>
+    <mergeCell ref="AC8:AI8"/>
+    <mergeCell ref="AJ8:AP8"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="A1:BR1"/>
     <mergeCell ref="A2:BR2"/>
     <mergeCell ref="A3:BR3"/>
@@ -10868,12 +10916,6 @@
     <mergeCell ref="AC9:AI9"/>
     <mergeCell ref="AJ9:AP9"/>
     <mergeCell ref="AQ9:AW9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="O8:U8"/>
-    <mergeCell ref="V8:AB8"/>
-    <mergeCell ref="AC8:AI8"/>
-    <mergeCell ref="AJ8:AP8"/>
-    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="L12:L22 L36:L46">
     <cfRule type="dataBar" priority="117">
@@ -11152,65 +11194,65 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="206"/>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="202" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
-      <c r="I2" s="207"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="207"/>
-      <c r="P2" s="207"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="207"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11252,65 +11294,65 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="206"/>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="202" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
-      <c r="I2" s="207"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="207"/>
-      <c r="P2" s="207"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="207"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11352,65 +11394,65 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="206"/>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="202" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
-      <c r="I2" s="207"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="207"/>
-      <c r="P2" s="207"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="202" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="207"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>
@@ -11452,65 +11494,65 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="206"/>
-      <c r="B1" s="206"/>
-      <c r="C1" s="206"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
+      <c r="M1" s="201"/>
     </row>
     <row r="2" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="202" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="207"/>
-      <c r="C2" s="207"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="207"/>
-      <c r="H2" s="207"/>
-      <c r="I2" s="207"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="207"/>
-      <c r="L2" s="207"/>
-      <c r="M2" s="207"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="207"/>
-      <c r="P2" s="207"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="202"/>
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="202"/>
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
     </row>
     <row r="3" spans="1:16" s="41" customFormat="1" ht="20.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="202" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="207"/>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="207"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="202"/>
+      <c r="I3" s="202"/>
+      <c r="J3" s="202"/>
+      <c r="K3" s="202"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="202"/>
+      <c r="N3" s="202"/>
+      <c r="O3" s="202"/>
+      <c r="P3" s="202"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="56"/>

</xml_diff>